<commit_message>
Seed, bias and test cases
</commit_message>
<xml_diff>
--- a/test/YANNL-walkthrough.xlsx
+++ b/test/YANNL-walkthrough.xlsx
@@ -5,24 +5,25 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MDeloison\_Never Backup\Cpp\YANNL-vc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MDeloison\_Never Backup\Cpp\YANNL-vc\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B28E576-980A-4350-9188-099F92889EF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8887BA26-9D01-433E-AA2C-0F74B08F09C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="8" xr2:uid="{3DE57AAC-3496-42F8-B681-7BA2B7FE7A12}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="10" xr2:uid="{3DE57AAC-3496-42F8-B681-7BA2B7FE7A12}"/>
   </bookViews>
   <sheets>
-    <sheet name="Standard" sheetId="1" r:id="rId1"/>
+    <sheet name="No bias" sheetId="1" r:id="rId1"/>
     <sheet name="Dropout 1.0 on HL" sheetId="5" r:id="rId2"/>
     <sheet name="Dropout 0.4 on HL" sheetId="4" r:id="rId3"/>
     <sheet name="Dropout 1.0 on IL" sheetId="7" r:id="rId4"/>
     <sheet name="Dropout 0.4 on IL" sheetId="8" r:id="rId5"/>
-    <sheet name="Bias" sheetId="10" r:id="rId6"/>
-    <sheet name="Momentum and bias" sheetId="9" r:id="rId7"/>
+    <sheet name="Normal" sheetId="10" r:id="rId6"/>
+    <sheet name="Momentum" sheetId="9" r:id="rId7"/>
     <sheet name="Softmax 2 outputs" sheetId="11" r:id="rId8"/>
     <sheet name="Softmax 3 outputs" sheetId="13" r:id="rId9"/>
     <sheet name="Class structure" sheetId="12" r:id="rId10"/>
+    <sheet name="Normal (2)" sheetId="16" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="102">
   <si>
     <t>i1</t>
   </si>
@@ -516,6 +517,12 @@
   <si>
     <t>d E total / d w8</t>
   </si>
+  <si>
+    <t>Seed</t>
+  </si>
+  <si>
+    <t>droppedNeuron</t>
+  </si>
 </sst>
 </file>
 
@@ -660,7 +667,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -750,32 +757,18 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2077,6 +2070,1283 @@
       <xdr:spPr>
         <a:xfrm flipV="1">
           <a:off x="4968240" y="2133600"/>
+          <a:ext cx="1684020" cy="853440"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Straight Arrow Connector 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7B1E4DE-765E-4749-9AAF-E31CE667E055}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1889760" y="975360"/>
+          <a:ext cx="1752600" cy="7620"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6096CF83-C871-4B57-AFDF-C1760EFB5FAB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1905000" y="1066800"/>
+          <a:ext cx="1661160" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6DA99E8-944F-4E4C-BEC2-A94D1A34BE95}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1889760" y="1066800"/>
+          <a:ext cx="1737360" cy="792480"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>525780</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CD7B857-48D5-4CA3-9380-E8DEB7C75666}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1866900" y="1943100"/>
+          <a:ext cx="1706880" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>541020</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37F9470C-68C7-41CF-8F68-C3A753C4C5D8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1874520" y="1127760"/>
+          <a:ext cx="1714500" cy="1844040"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E722AD9A-1456-4598-B627-79F57EAE0363}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1920240" y="2133600"/>
+          <a:ext cx="1684020" cy="853440"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F271C2A-A975-47BA-87AF-FA8A27828936}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4937760" y="975360"/>
+          <a:ext cx="1752600" cy="7620"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{856DCAF2-191F-40EE-96CC-A8E77FD3B305}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4953000" y="1066800"/>
+          <a:ext cx="1661160" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Arrow Connector 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32C4F8B7-04C8-4EDE-AE34-7E9B0D244D97}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4937760" y="1066800"/>
+          <a:ext cx="1737360" cy="792480"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>525780</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44A11474-02C7-4549-9E91-5BD112DD9ACC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4914900" y="1943100"/>
+          <a:ext cx="1706880" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>541020</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Straight Arrow Connector 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76E479A2-4986-41B2-BC0D-15E4B43659CF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4922520" y="1127760"/>
+          <a:ext cx="1714500" cy="1844040"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2F1D07F-55EE-4AF5-B986-A5E58EE4F009}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4968240" y="2133600"/>
+          <a:ext cx="1684020" cy="853440"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8572059A-5989-4222-A404-D4764468D1E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1889760" y="4450080"/>
+          <a:ext cx="1752600" cy="7620"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1743506B-BC48-4828-B182-F6C2930C315C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1905000" y="4541520"/>
+          <a:ext cx="1661160" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42323510-04D2-409B-9547-12C9E20E1155}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1889760" y="4541520"/>
+          <a:ext cx="1737360" cy="792480"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>525780</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Straight Arrow Connector 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{939F040C-047E-419D-91B2-9172C5CA3869}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1866900" y="5417820"/>
+          <a:ext cx="1706880" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>541020</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Straight Arrow Connector 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A1E9DA5-9367-412B-91E1-6A40E3AB5B93}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1874520" y="4602480"/>
+          <a:ext cx="1714500" cy="1844040"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Arrow Connector 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57F2DAC5-A83C-4973-BEB2-BC767E7B4069}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1920240" y="5608320"/>
+          <a:ext cx="1684020" cy="853440"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Straight Arrow Connector 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{669C41A0-E34F-4C6D-9BB8-C3904B7BC432}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4937760" y="4450080"/>
+          <a:ext cx="1752600" cy="7620"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Straight Arrow Connector 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97DF429E-EB8F-4E5B-99FE-F245BE08A27B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4953000" y="4541520"/>
+          <a:ext cx="1661160" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Straight Arrow Connector 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{359B66D1-084B-4860-9158-D64866170D43}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4937760" y="4541520"/>
+          <a:ext cx="1737360" cy="792480"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>525780</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Straight Arrow Connector 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A11AF76-F1A8-4795-8A0E-D46AB8C8F6D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4914900" y="5417820"/>
+          <a:ext cx="1706880" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>541020</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1ED2C8A-B6BB-46AE-A164-E5F3B9C1BF1D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4922520" y="4602480"/>
+          <a:ext cx="1714500" cy="1844040"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Straight Arrow Connector 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A6FF3F2-2B32-44E4-A437-E11DF5FB866C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4968240" y="5608320"/>
           <a:ext cx="1684020" cy="853440"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -16206,10 +17476,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E61986C2-8653-4DD1-B246-0EFA6CD3A7C8}">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16319,284 +17589,778 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
-        <v>78</v>
+        <v>101</v>
       </c>
       <c r="B11" t="s">
-        <v>78</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="17" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B16" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C16" s="17" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="C16" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="B17" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="B22" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="C22" t="s">
-        <v>75</v>
+        <v>74</v>
+      </c>
+      <c r="B22" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="B23" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="B25" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="C25" t="s">
-        <v>78</v>
+        <v>77</v>
+      </c>
+      <c r="B25" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B26" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B28" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B28" s="17" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B30" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C30" s="17" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B29" s="18" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B31" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C31" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B35" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="C35" t="s">
-        <v>75</v>
+      <c r="B35" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B37" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B38" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="C38" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B41" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B41" s="17" t="s">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B44" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="C41" s="17" t="s">
+      <c r="C44" s="17" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B42" s="18" t="s">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B45" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C45" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B43" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B44" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B45" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>73</v>
-      </c>
-      <c r="C46" s="20" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>74</v>
-      </c>
-      <c r="C47" s="20" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B48" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="C48" t="s">
-        <v>75</v>
+      <c r="B48" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C49" s="20" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>77</v>
+        <v>74</v>
+      </c>
+      <c r="C50" s="20" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B51" s="18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C51" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
+        <v>76</v>
+      </c>
+      <c r="C52" s="20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B55" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C55" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
         <v>79</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB38494-A661-4DF2-BD0C-434142B41BB0}">
+  <dimension ref="B2:Q37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I4" activeCellId="1" sqref="D4:E16 I4:J17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="35"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B2" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="C5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="35">
+        <v>0.14938799999999999</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="35">
+        <v>0.27986</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="C6" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="G6" s="6">
+        <f>C6*E5+C12*E10+C18*D14</f>
+        <v>0.36510900000000002</v>
+      </c>
+      <c r="H6" s="6">
+        <f>1/(1+EXP(-G6))</f>
+        <v>0.59027661385405872</v>
+      </c>
+      <c r="L6" s="6">
+        <f>H6*J5+H12*J10+H18*I14</f>
+        <v>0.7578963990901505</v>
+      </c>
+      <c r="M6" s="6">
+        <f>1/(1+EXP(-L6))</f>
+        <v>0.68089684513106064</v>
+      </c>
+      <c r="O6" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="P6" s="6">
+        <f>(O6-M6)^2</f>
+        <v>0.45010257680681037</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="D7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="35">
+        <v>0.24930099999999999</v>
+      </c>
+      <c r="G7" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="35">
+        <v>0.53228200000000003</v>
+      </c>
+      <c r="L7" s="35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="G8" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="L8" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="G9" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="L9" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q9" s="6">
+        <f>(P6+P12)/2</f>
+        <v>0.24540569717207955</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="D10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="35">
+        <v>0.19877600000000001</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="35">
+        <v>0.32913799999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="C11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="C12" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="35">
+        <v>0.29860199999999998</v>
+      </c>
+      <c r="G12" s="6">
+        <f>C6*E7+C12*E12+C18*E15</f>
+        <v>0.37834224999999999</v>
+      </c>
+      <c r="H12" s="6">
+        <f>1/(1+EXP(-G12))</f>
+        <v>0.59347321165272204</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" s="35">
+        <v>0.58247599999999999</v>
+      </c>
+      <c r="L12" s="6">
+        <f>H6*J7+H12*J12+H18*J15</f>
+        <v>1.3143235190060971</v>
+      </c>
+      <c r="M12" s="6">
+        <f>1/(1+EXP(-L12))</f>
+        <v>0.78823573771019617</v>
+      </c>
+      <c r="O12" s="6">
+        <v>0.99</v>
+      </c>
+      <c r="P12" s="6">
+        <f>(O12-M12)^2</f>
+        <v>4.070881753734875E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="D14" s="35">
+        <v>0.33776200000000001</v>
+      </c>
+      <c r="I14" s="35">
+        <v>0.39736700000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="D15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="35">
+        <v>0.33601700000000001</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J15" s="35">
+        <v>0.65444599999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="L16" s="7"/>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L17" s="8"/>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C18" s="6">
+        <v>1</v>
+      </c>
+      <c r="H18" s="6">
+        <v>1</v>
+      </c>
+      <c r="L18" s="7"/>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="L19" s="7"/>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B22" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C24" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="35">
+        <f>E5-0.5*G25*C25</f>
+        <v>0.1492497299124918</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J24" s="35">
+        <f>J5-0.5*L$25*H6</f>
+        <v>0.23683768744315331</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N24" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="O24" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C25" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="G25" s="6">
+        <f>H6*(1-H6)*H25</f>
+        <v>5.5308035003278936E-3</v>
+      </c>
+      <c r="H25" s="6">
+        <f>J5*L25+J7*L31</f>
+        <v>2.2868722179006117E-2</v>
+      </c>
+      <c r="L25" s="6">
+        <f>M25*N25</f>
+        <v>0.14577000527242168</v>
+      </c>
+      <c r="M25" s="6">
+        <f>M6*(1-M6)</f>
+        <v>0.21727633142162905</v>
+      </c>
+      <c r="N25" s="6">
+        <f>-(O25-M6)</f>
+        <v>0.67089684513106063</v>
+      </c>
+      <c r="O25" s="6">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="D26" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="35">
+        <f>E7-0.5*G31*C25</f>
+        <v>0.24912993555585886</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J26" s="35">
+        <f>J7-0.5*L$31*H6</f>
+        <v>0.54222182221202797</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="D29" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="35">
+        <f>E10-0.5*G25*C31</f>
+        <v>0.19849945982498363</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J29" s="35">
+        <f>J10-0.5*L$25*H12</f>
+        <v>0.28588270340417082</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C30" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M30" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N30" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="O30" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C31" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="35">
+        <f>E12-0.5*G31*C31</f>
+        <v>0.2982598711117177</v>
+      </c>
+      <c r="G31" s="6">
+        <f>H12*(1-H12)*H31</f>
+        <v>6.8425777656451175E-3</v>
+      </c>
+      <c r="H31" s="6">
+        <f>J10*L25+J12*L31</f>
+        <v>2.836151672318088E-2</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J31" s="35">
+        <f>J12-0.5*L$31*H12</f>
+        <v>0.59246965055802081</v>
+      </c>
+      <c r="L31" s="6">
+        <f>M31*N31</f>
+        <v>-3.3678522844157441E-2</v>
+      </c>
+      <c r="M31" s="6">
+        <f>M12*(1-M12)</f>
+        <v>0.166920159506659</v>
+      </c>
+      <c r="N31" s="6">
+        <f>-(O31-M12)</f>
+        <v>-0.20176426228980382</v>
+      </c>
+      <c r="O31" s="6">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="33" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="D33" s="35">
+        <f>D14-0.5*G25*C18</f>
+        <v>0.33499659824983608</v>
+      </c>
+      <c r="I33" s="35">
+        <f>I14-0.5*L25*H18</f>
+        <v>0.32448199736378919</v>
+      </c>
+    </row>
+    <row r="34" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="D34" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E34" s="35">
+        <f>E15-0.5*G$31*C18</f>
+        <v>0.33259571111717745</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J34" s="35">
+        <f>J15-0.5*L$31*H18</f>
+        <v>0.67128526142207867</v>
+      </c>
+    </row>
+    <row r="35" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="L35" s="7"/>
+    </row>
+    <row r="36" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C36" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L36" s="8"/>
+    </row>
+    <row r="37" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C37" s="6">
+        <v>1</v>
+      </c>
+      <c r="H37" s="6">
+        <v>1</v>
+      </c>
+      <c r="L37" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -16605,7 +18369,7 @@
   <dimension ref="B2:S37"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16825,6 +18589,14 @@
         <v>40</v>
       </c>
     </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="D14" s="5">
+        <v>0.35</v>
+      </c>
+      <c r="K14" s="5">
+        <v>0.6</v>
+      </c>
+    </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.3">
       <c r="D15" s="4" t="s">
         <v>2</v>
@@ -16877,7 +18649,7 @@
       </c>
       <c r="E24" s="5">
         <f>E5-0.5*G25*C25</f>
-        <v>0.14988670296588974</v>
+        <v>0.15</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>43</v>
@@ -16913,8 +18685,8 @@
         <v>0.05</v>
       </c>
       <c r="G25" s="6">
-        <f>H6*(1-H6)*H25</f>
-        <v>4.5318813644100332E-3</v>
+        <f>J6*(1-J6)*H25</f>
+        <v>0</v>
       </c>
       <c r="H25" s="6">
         <f>L5*N25+L7*N31</f>
@@ -16945,7 +18717,7 @@
       </c>
       <c r="E26" s="5">
         <f>E7-0.5*G31*C25</f>
-        <v>0.24986698024323636</v>
+        <v>0.25</v>
       </c>
       <c r="K26" s="4" t="s">
         <v>17</v>
@@ -16961,7 +18733,7 @@
       </c>
       <c r="E29" s="5">
         <f>E10-0.5*G25*C31</f>
-        <v>0.1997734059317795</v>
+        <v>0.2</v>
       </c>
       <c r="K29" s="4" t="s">
         <v>18</v>
@@ -17006,11 +18778,11 @@
       </c>
       <c r="E31" s="5">
         <f>E12-0.5*G31*C31</f>
-        <v>0.29973396048647272</v>
+        <v>0.3</v>
       </c>
       <c r="G31" s="6">
-        <f>H12*(1-H12)*H31</f>
-        <v>5.32079027054491E-3</v>
+        <f>J12*(1-J12)*H31</f>
+        <v>0</v>
       </c>
       <c r="H31" s="6">
         <f>L10*N25+L12*N31</f>
@@ -17042,18 +18814,30 @@
         <v>0.99</v>
       </c>
     </row>
+    <row r="33" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="D33" s="5">
+        <f>D14-0.5*G25*C18</f>
+        <v>0.35</v>
+      </c>
+      <c r="K33" s="5">
+        <f>K14-0.5*N25*J18</f>
+        <v>0.52728592739432345</v>
+      </c>
+    </row>
     <row r="34" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D34" s="4" t="s">
         <v>2</v>
       </c>
       <c r="E34" s="5">
+        <f>E15-0.5*G$31*C18</f>
         <v>0.35</v>
       </c>
       <c r="K34" s="4" t="s">
         <v>3</v>
       </c>
       <c r="L34" s="5">
-        <v>0.6</v>
+        <f>L15-0.5*N$31*J18</f>
+        <v>0.63939020521808554</v>
       </c>
     </row>
     <row r="35" spans="3:14" x14ac:dyDescent="0.3">
@@ -17089,12 +18873,14 @@
   <dimension ref="B2:S37"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="8" width="8.88671875" style="5"/>
+    <col min="1" max="4" width="8.88671875" style="5"/>
+    <col min="5" max="5" width="8.88671875" style="5" customWidth="1"/>
+    <col min="6" max="8" width="8.88671875" style="5"/>
     <col min="11" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
@@ -17108,6 +18894,13 @@
       <c r="H2" s="5">
         <v>0.4</v>
       </c>
+      <c r="J2" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="K2" s="36">
+        <v>1199908899</v>
+      </c>
+      <c r="L2" s="36"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.3">
       <c r="C5" s="3" t="s">
@@ -17310,6 +19103,14 @@
         <v>40</v>
       </c>
     </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="D14" s="5">
+        <v>0.35</v>
+      </c>
+      <c r="K14" s="5">
+        <v>0.6</v>
+      </c>
+    </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.3">
       <c r="D15" s="4" t="s">
         <v>2</v>
@@ -17362,7 +19163,7 @@
       </c>
       <c r="E24" s="5">
         <f>E5-0.5*G25*C25</f>
-        <v>0.14978867293154918</v>
+        <v>0.15</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>43</v>
@@ -17398,8 +19199,8 @@
         <v>0.05</v>
       </c>
       <c r="G25" s="6">
-        <f>H6*(1-H6)*H25</f>
-        <v>8.4530827380319817E-3</v>
+        <f>J6*(1-J6)*H25</f>
+        <v>0</v>
       </c>
       <c r="H25" s="6">
         <f>L5*N25+L7*N31</f>
@@ -17430,7 +19231,7 @@
       </c>
       <c r="E26" s="5">
         <f>E7-0.5*G31*C25</f>
-        <v>0.24975975678115567</v>
+        <v>0.24999484220906687</v>
       </c>
       <c r="K26" s="4" t="s">
         <v>17</v>
@@ -17446,7 +19247,7 @@
       </c>
       <c r="E29" s="5">
         <f>E10-0.5*G25*C31</f>
-        <v>0.19957734586309842</v>
+        <v>0.2</v>
       </c>
       <c r="K29" s="4" t="s">
         <v>18</v>
@@ -17491,11 +19292,11 @@
       </c>
       <c r="E31" s="5">
         <f>E12-0.5*G31*C31</f>
-        <v>0.29951951356231132</v>
+        <v>0.29998968441813373</v>
       </c>
       <c r="G31" s="6">
-        <f>H12*(1-H12)*H31</f>
-        <v>9.6097287537734426E-3</v>
+        <f>J12*(1-J12)*H31</f>
+        <v>2.0631163732564317E-4</v>
       </c>
       <c r="H31" s="6">
         <f>L10*N25+L12*N31</f>
@@ -17528,18 +19329,30 @@
         <v>0.99</v>
       </c>
     </row>
+    <row r="33" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="D33" s="5">
+        <f>D14-0.5*G25*C18</f>
+        <v>0.35</v>
+      </c>
+      <c r="K33" s="5">
+        <f>K14-0.5*N25*J18</f>
+        <v>0.52979981300434353</v>
+      </c>
+    </row>
     <row r="34" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D34" s="4" t="s">
         <v>2</v>
       </c>
       <c r="E34" s="5">
-        <v>0.35</v>
+        <f>E15-0.5*G$31*C18</f>
+        <v>0.34989684418133715</v>
       </c>
       <c r="K34" s="4" t="s">
         <v>3</v>
       </c>
       <c r="L34" s="5">
-        <v>0.6</v>
+        <f>L15-0.5*N$31*J18</f>
+        <v>0.62112882793963775</v>
       </c>
     </row>
     <row r="35" spans="3:14" x14ac:dyDescent="0.3">
@@ -17564,6 +19377,9 @@
       <c r="N37" s="7"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="K2:L2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -17575,7 +19391,7 @@
   <dimension ref="B2:S37"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17810,6 +19626,12 @@
     <row r="14" spans="2:19" x14ac:dyDescent="0.3">
       <c r="D14"/>
       <c r="E14"/>
+      <c r="F14" s="5">
+        <v>0.35</v>
+      </c>
+      <c r="K14" s="5">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.3">
       <c r="D15"/>
@@ -18066,18 +19888,30 @@
         <v>0.99</v>
       </c>
     </row>
+    <row r="33" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="F33" s="5">
+        <f>F14-0.5*I25*E18</f>
+        <v>0.34560858652315335</v>
+      </c>
+      <c r="K33" s="5">
+        <f>K14-0.5*N25*J18</f>
+        <v>0.53062521649476946</v>
+      </c>
+    </row>
     <row r="34" spans="5:14" x14ac:dyDescent="0.3">
       <c r="F34" s="4" t="s">
         <v>2</v>
       </c>
       <c r="G34" s="5">
-        <v>0.35</v>
+        <f>G15-0.5*I$31*E18</f>
+        <v>0.34500121313266602</v>
       </c>
       <c r="K34" s="4" t="s">
         <v>3</v>
       </c>
       <c r="L34" s="5">
-        <v>0.6</v>
+        <f>L15-0.5*N$31*J18</f>
+        <v>0.61928159463357346</v>
       </c>
     </row>
     <row r="35" spans="5:14" x14ac:dyDescent="0.3">
@@ -18113,12 +19947,14 @@
   <dimension ref="B2:S37"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="5"/>
+    <col min="1" max="10" width="8.88671875" style="5"/>
+    <col min="11" max="11" width="8.88671875" style="5" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.3">
@@ -18131,6 +19967,12 @@
       <c r="H2" s="5">
         <v>0.4</v>
       </c>
+      <c r="J2" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="K2" s="5">
+        <v>20</v>
+      </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.3">
       <c r="C5" s="3" t="s">
@@ -18355,6 +20197,12 @@
     <row r="14" spans="2:19" x14ac:dyDescent="0.3">
       <c r="D14"/>
       <c r="E14"/>
+      <c r="F14" s="5">
+        <v>0.35</v>
+      </c>
+      <c r="K14" s="5">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.3">
       <c r="D15"/>
@@ -18612,19 +20460,32 @@
         <v>0.99</v>
       </c>
     </row>
+    <row r="33" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="F33" s="5">
+        <f>F14-0.5*I25*E18</f>
+        <v>0.34561616516778654</v>
+      </c>
+      <c r="K33" s="5">
+        <f>K14-0.5*N25*J18</f>
+        <v>0.53077461314000995</v>
+      </c>
+    </row>
     <row r="34" spans="5:14" x14ac:dyDescent="0.3">
       <c r="F34" s="4" t="s">
         <v>2</v>
       </c>
       <c r="G34" s="5">
-        <v>0.35</v>
+        <f>G15-0.5*I$31*E18</f>
+        <v>0.34502697617289696</v>
       </c>
       <c r="K34" s="4" t="s">
         <v>3</v>
       </c>
       <c r="L34" s="5">
-        <v>0.6</v>
-      </c>
+        <f>L15-0.5*N$31*J18</f>
+        <v>0.61900541655425223</v>
+      </c>
+      <c r="M34" s="4"/>
     </row>
     <row r="35" spans="5:14" x14ac:dyDescent="0.3">
       <c r="N35" s="7"/>
@@ -18659,7 +20520,7 @@
   <dimension ref="B2:Q37"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18712,7 +20573,7 @@
         <v>0.05</v>
       </c>
       <c r="G6" s="6">
-        <f>C6*E5+C12*E10+C18*E15</f>
+        <f>C6*E5+C12*E10+C18*D14</f>
         <v>0.3775</v>
       </c>
       <c r="H6" s="6">
@@ -18720,7 +20581,7 @@
         <v>0.59326999210718723</v>
       </c>
       <c r="L6" s="6">
-        <f>H6*J5+H12*J10+H18*J15</f>
+        <f>H6*J5+H12*J10+H18*I14</f>
         <v>1.10590596705977</v>
       </c>
       <c r="M6" s="6">
@@ -19127,7 +20988,7 @@
   <dimension ref="B2:AH37"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19216,7 +21077,7 @@
         <v>0.05</v>
       </c>
       <c r="G6" s="6">
-        <f>C6*E5+C12*E10+C18*E15</f>
+        <f>C6*E5+C12*E10+C18*D14</f>
         <v>0.3775</v>
       </c>
       <c r="H6" s="6">
@@ -19224,7 +21085,7 @@
         <v>0.59326999210718723</v>
       </c>
       <c r="L6" s="6">
-        <f>H6*J5+H12*J10+H18*J15</f>
+        <f>H6*J5+H12*J10+H18*I14</f>
         <v>1.10590596705977</v>
       </c>
       <c r="M6" s="6">
@@ -19948,8 +21809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ACBA4E1-69CC-4018-9E79-34FECB1B09E7}">
   <dimension ref="A1:R59"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20220,7 +22081,7 @@
         <v>0.05</v>
       </c>
       <c r="H28" s="6">
-        <f>D28*F27+D34*F32+D40*F37</f>
+        <f>D28*F27+D34*F32+D40*E36</f>
         <v>0.3775</v>
       </c>
       <c r="I28" s="6">
@@ -20228,7 +22089,7 @@
         <v>0.59326999210718723</v>
       </c>
       <c r="M28" s="6">
-        <f>I28*K27+I34*K32+I40*K37</f>
+        <f>I28*K27+I34*K32+I40*J36</f>
         <v>1.10590596705977</v>
       </c>
       <c r="N28" s="6">
@@ -20579,12 +22440,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B19">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>$B$11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>$B$15</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20601,8 +22462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F931B127-BA82-4815-97AD-3B76F9C00B88}">
   <dimension ref="A1:T37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S24" sqref="S24"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20702,7 +22563,7 @@
         <v>0.05</v>
       </c>
       <c r="F6" s="6">
-        <f>B6*D5+B12*D10+B18*D15</f>
+        <f>B6*D5+B12*D10+B18*C14</f>
         <v>0.3775</v>
       </c>
       <c r="G6" s="6">
@@ -21277,12 +23138,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="S24:S25">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>$B$15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S23">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>$B$11</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
MLPRegressor, iris flower classification test
</commit_message>
<xml_diff>
--- a/test/YANNL-walkthrough.xlsx
+++ b/test/YANNL-walkthrough.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MDeloison\_Never Backup\Cpp\YANNL-vc\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83FE2F3-E4C2-4FA8-87AE-B04C02B303D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BAD3799-FA42-461B-9A17-83B60CF0AB26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="5" xr2:uid="{3DE57AAC-3496-42F8-B681-7BA2B7FE7A12}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="5" xr2:uid="{3DE57AAC-3496-42F8-B681-7BA2B7FE7A12}"/>
   </bookViews>
   <sheets>
     <sheet name="No bias" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,9 @@
     <sheet name="Softmax 3 outputs" sheetId="13" r:id="rId9"/>
     <sheet name="Class structure" sheetId="12" r:id="rId10"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId11"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -15450,6 +15453,2129 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="A2">
+            <v>5.0999999999999996</v>
+          </cell>
+          <cell r="B2">
+            <v>3.5</v>
+          </cell>
+          <cell r="C2">
+            <v>1.4</v>
+          </cell>
+          <cell r="D2">
+            <v>0.2</v>
+          </cell>
+          <cell r="E2" t="str">
+            <v>iris_setosa</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3">
+            <v>4.9000000000000004</v>
+          </cell>
+          <cell r="B3">
+            <v>3</v>
+          </cell>
+          <cell r="C3">
+            <v>1.4</v>
+          </cell>
+          <cell r="D3">
+            <v>0.2</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>4.7</v>
+          </cell>
+          <cell r="B4">
+            <v>3.2</v>
+          </cell>
+          <cell r="C4">
+            <v>1.3</v>
+          </cell>
+          <cell r="D4">
+            <v>0.2</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>4.5999999999999996</v>
+          </cell>
+          <cell r="B5">
+            <v>3.1</v>
+          </cell>
+          <cell r="C5">
+            <v>1.5</v>
+          </cell>
+          <cell r="D5">
+            <v>0.2</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6">
+            <v>5</v>
+          </cell>
+          <cell r="B6">
+            <v>3.6</v>
+          </cell>
+          <cell r="C6">
+            <v>1.4</v>
+          </cell>
+          <cell r="D6">
+            <v>0.2</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7">
+            <v>5.4</v>
+          </cell>
+          <cell r="B7">
+            <v>3.9</v>
+          </cell>
+          <cell r="C7">
+            <v>1.7</v>
+          </cell>
+          <cell r="D7">
+            <v>0.4</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8">
+            <v>4.5999999999999996</v>
+          </cell>
+          <cell r="B8">
+            <v>3.4</v>
+          </cell>
+          <cell r="C8">
+            <v>1.4</v>
+          </cell>
+          <cell r="D8">
+            <v>0.3</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9">
+            <v>5</v>
+          </cell>
+          <cell r="B9">
+            <v>3.4</v>
+          </cell>
+          <cell r="C9">
+            <v>1.5</v>
+          </cell>
+          <cell r="D9">
+            <v>0.2</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10">
+            <v>4.4000000000000004</v>
+          </cell>
+          <cell r="B10">
+            <v>2.9</v>
+          </cell>
+          <cell r="C10">
+            <v>1.4</v>
+          </cell>
+          <cell r="D10">
+            <v>0.2</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11">
+            <v>4.9000000000000004</v>
+          </cell>
+          <cell r="B11">
+            <v>3.1</v>
+          </cell>
+          <cell r="C11">
+            <v>1.5</v>
+          </cell>
+          <cell r="D11">
+            <v>0.1</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12">
+            <v>5.4</v>
+          </cell>
+          <cell r="B12">
+            <v>3.7</v>
+          </cell>
+          <cell r="C12">
+            <v>1.5</v>
+          </cell>
+          <cell r="D12">
+            <v>0.2</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13">
+            <v>4.8</v>
+          </cell>
+          <cell r="B13">
+            <v>3.4</v>
+          </cell>
+          <cell r="C13">
+            <v>1.6</v>
+          </cell>
+          <cell r="D13">
+            <v>0.2</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14">
+            <v>4.8</v>
+          </cell>
+          <cell r="B14">
+            <v>3</v>
+          </cell>
+          <cell r="C14">
+            <v>1.4</v>
+          </cell>
+          <cell r="D14">
+            <v>0.1</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15">
+            <v>4.3</v>
+          </cell>
+          <cell r="B15">
+            <v>3</v>
+          </cell>
+          <cell r="C15">
+            <v>1.1000000000000001</v>
+          </cell>
+          <cell r="D15">
+            <v>0.1</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16">
+            <v>5.8</v>
+          </cell>
+          <cell r="B16">
+            <v>4</v>
+          </cell>
+          <cell r="C16">
+            <v>1.2</v>
+          </cell>
+          <cell r="D16">
+            <v>0.2</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17">
+            <v>5.7</v>
+          </cell>
+          <cell r="B17">
+            <v>4.4000000000000004</v>
+          </cell>
+          <cell r="C17">
+            <v>1.5</v>
+          </cell>
+          <cell r="D17">
+            <v>0.4</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18">
+            <v>5.4</v>
+          </cell>
+          <cell r="B18">
+            <v>3.9</v>
+          </cell>
+          <cell r="C18">
+            <v>1.3</v>
+          </cell>
+          <cell r="D18">
+            <v>0.4</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19">
+            <v>5.0999999999999996</v>
+          </cell>
+          <cell r="B19">
+            <v>3.5</v>
+          </cell>
+          <cell r="C19">
+            <v>1.4</v>
+          </cell>
+          <cell r="D19">
+            <v>0.3</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20">
+            <v>5.7</v>
+          </cell>
+          <cell r="B20">
+            <v>3.8</v>
+          </cell>
+          <cell r="C20">
+            <v>1.7</v>
+          </cell>
+          <cell r="D20">
+            <v>0.3</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21">
+            <v>5.0999999999999996</v>
+          </cell>
+          <cell r="B21">
+            <v>3.8</v>
+          </cell>
+          <cell r="C21">
+            <v>1.5</v>
+          </cell>
+          <cell r="D21">
+            <v>0.3</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22">
+            <v>5.4</v>
+          </cell>
+          <cell r="B22">
+            <v>3.4</v>
+          </cell>
+          <cell r="C22">
+            <v>1.7</v>
+          </cell>
+          <cell r="D22">
+            <v>0.2</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23">
+            <v>5.0999999999999996</v>
+          </cell>
+          <cell r="B23">
+            <v>3.7</v>
+          </cell>
+          <cell r="C23">
+            <v>1.5</v>
+          </cell>
+          <cell r="D23">
+            <v>0.4</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="A24">
+            <v>4.5999999999999996</v>
+          </cell>
+          <cell r="B24">
+            <v>3.6</v>
+          </cell>
+          <cell r="C24">
+            <v>1</v>
+          </cell>
+          <cell r="D24">
+            <v>0.2</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="A25">
+            <v>5.0999999999999996</v>
+          </cell>
+          <cell r="B25">
+            <v>3.3</v>
+          </cell>
+          <cell r="C25">
+            <v>1.7</v>
+          </cell>
+          <cell r="D25">
+            <v>0.5</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="A26">
+            <v>4.8</v>
+          </cell>
+          <cell r="B26">
+            <v>3.4</v>
+          </cell>
+          <cell r="C26">
+            <v>1.9</v>
+          </cell>
+          <cell r="D26">
+            <v>0.2</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="A27">
+            <v>5</v>
+          </cell>
+          <cell r="B27">
+            <v>3</v>
+          </cell>
+          <cell r="C27">
+            <v>1.6</v>
+          </cell>
+          <cell r="D27">
+            <v>0.2</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28">
+            <v>5</v>
+          </cell>
+          <cell r="B28">
+            <v>3.4</v>
+          </cell>
+          <cell r="C28">
+            <v>1.6</v>
+          </cell>
+          <cell r="D28">
+            <v>0.4</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="A29">
+            <v>5.2</v>
+          </cell>
+          <cell r="B29">
+            <v>3.5</v>
+          </cell>
+          <cell r="C29">
+            <v>1.5</v>
+          </cell>
+          <cell r="D29">
+            <v>0.2</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="A30">
+            <v>5.2</v>
+          </cell>
+          <cell r="B30">
+            <v>3.4</v>
+          </cell>
+          <cell r="C30">
+            <v>1.4</v>
+          </cell>
+          <cell r="D30">
+            <v>0.2</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="A31">
+            <v>4.7</v>
+          </cell>
+          <cell r="B31">
+            <v>3.2</v>
+          </cell>
+          <cell r="C31">
+            <v>1.6</v>
+          </cell>
+          <cell r="D31">
+            <v>0.2</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="A32">
+            <v>4.8</v>
+          </cell>
+          <cell r="B32">
+            <v>3.1</v>
+          </cell>
+          <cell r="C32">
+            <v>1.6</v>
+          </cell>
+          <cell r="D32">
+            <v>0.2</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="A33">
+            <v>5.4</v>
+          </cell>
+          <cell r="B33">
+            <v>3.4</v>
+          </cell>
+          <cell r="C33">
+            <v>1.5</v>
+          </cell>
+          <cell r="D33">
+            <v>0.4</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="A34">
+            <v>5.2</v>
+          </cell>
+          <cell r="B34">
+            <v>4.0999999999999996</v>
+          </cell>
+          <cell r="C34">
+            <v>1.5</v>
+          </cell>
+          <cell r="D34">
+            <v>0.1</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="A35">
+            <v>5.5</v>
+          </cell>
+          <cell r="B35">
+            <v>4.2</v>
+          </cell>
+          <cell r="C35">
+            <v>1.4</v>
+          </cell>
+          <cell r="D35">
+            <v>0.2</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="A36">
+            <v>4.9000000000000004</v>
+          </cell>
+          <cell r="B36">
+            <v>3.1</v>
+          </cell>
+          <cell r="C36">
+            <v>1.5</v>
+          </cell>
+          <cell r="D36">
+            <v>0.1</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="A37">
+            <v>5</v>
+          </cell>
+          <cell r="B37">
+            <v>3.2</v>
+          </cell>
+          <cell r="C37">
+            <v>1.2</v>
+          </cell>
+          <cell r="D37">
+            <v>0.2</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="A38">
+            <v>5.5</v>
+          </cell>
+          <cell r="B38">
+            <v>3.5</v>
+          </cell>
+          <cell r="C38">
+            <v>1.3</v>
+          </cell>
+          <cell r="D38">
+            <v>0.2</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="A39">
+            <v>4.9000000000000004</v>
+          </cell>
+          <cell r="B39">
+            <v>3.1</v>
+          </cell>
+          <cell r="C39">
+            <v>1.5</v>
+          </cell>
+          <cell r="D39">
+            <v>0.1</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="A40">
+            <v>4.4000000000000004</v>
+          </cell>
+          <cell r="B40">
+            <v>3</v>
+          </cell>
+          <cell r="C40">
+            <v>1.3</v>
+          </cell>
+          <cell r="D40">
+            <v>0.2</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="A41">
+            <v>5.0999999999999996</v>
+          </cell>
+          <cell r="B41">
+            <v>3.4</v>
+          </cell>
+          <cell r="C41">
+            <v>1.5</v>
+          </cell>
+          <cell r="D41">
+            <v>0.2</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="A42">
+            <v>5</v>
+          </cell>
+          <cell r="B42">
+            <v>3.5</v>
+          </cell>
+          <cell r="C42">
+            <v>1.3</v>
+          </cell>
+          <cell r="D42">
+            <v>0.3</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="A43">
+            <v>4.5</v>
+          </cell>
+          <cell r="B43">
+            <v>2.2999999999999998</v>
+          </cell>
+          <cell r="C43">
+            <v>1.3</v>
+          </cell>
+          <cell r="D43">
+            <v>0.3</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="A44">
+            <v>4.4000000000000004</v>
+          </cell>
+          <cell r="B44">
+            <v>3.2</v>
+          </cell>
+          <cell r="C44">
+            <v>1.3</v>
+          </cell>
+          <cell r="D44">
+            <v>0.2</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="A45">
+            <v>5</v>
+          </cell>
+          <cell r="B45">
+            <v>3.5</v>
+          </cell>
+          <cell r="C45">
+            <v>1.6</v>
+          </cell>
+          <cell r="D45">
+            <v>0.6</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="A46">
+            <v>5.0999999999999996</v>
+          </cell>
+          <cell r="B46">
+            <v>3.8</v>
+          </cell>
+          <cell r="C46">
+            <v>1.9</v>
+          </cell>
+          <cell r="D46">
+            <v>0.4</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="A47">
+            <v>4.8</v>
+          </cell>
+          <cell r="B47">
+            <v>3</v>
+          </cell>
+          <cell r="C47">
+            <v>1.4</v>
+          </cell>
+          <cell r="D47">
+            <v>0.3</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="A48">
+            <v>5.0999999999999996</v>
+          </cell>
+          <cell r="B48">
+            <v>3.8</v>
+          </cell>
+          <cell r="C48">
+            <v>1.6</v>
+          </cell>
+          <cell r="D48">
+            <v>0.2</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="A49">
+            <v>4.5999999999999996</v>
+          </cell>
+          <cell r="B49">
+            <v>3.2</v>
+          </cell>
+          <cell r="C49">
+            <v>1.4</v>
+          </cell>
+          <cell r="D49">
+            <v>0.2</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="A50">
+            <v>5.3</v>
+          </cell>
+          <cell r="B50">
+            <v>3.7</v>
+          </cell>
+          <cell r="C50">
+            <v>1.5</v>
+          </cell>
+          <cell r="D50">
+            <v>0.2</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="A51">
+            <v>5</v>
+          </cell>
+          <cell r="B51">
+            <v>3.3</v>
+          </cell>
+          <cell r="C51">
+            <v>1.4</v>
+          </cell>
+          <cell r="D51">
+            <v>0.2</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="A52">
+            <v>7</v>
+          </cell>
+          <cell r="B52">
+            <v>3.2</v>
+          </cell>
+          <cell r="C52">
+            <v>4.7</v>
+          </cell>
+          <cell r="D52">
+            <v>1.4</v>
+          </cell>
+          <cell r="E52" t="str">
+            <v>iris_versicolor</v>
+          </cell>
+        </row>
+        <row r="53">
+          <cell r="A53">
+            <v>6.4</v>
+          </cell>
+          <cell r="B53">
+            <v>3.2</v>
+          </cell>
+          <cell r="C53">
+            <v>4.5</v>
+          </cell>
+          <cell r="D53">
+            <v>1.5</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="A54">
+            <v>6.9</v>
+          </cell>
+          <cell r="B54">
+            <v>3.1</v>
+          </cell>
+          <cell r="C54">
+            <v>4.9000000000000004</v>
+          </cell>
+          <cell r="D54">
+            <v>1.5</v>
+          </cell>
+        </row>
+        <row r="55">
+          <cell r="A55">
+            <v>5.5</v>
+          </cell>
+          <cell r="B55">
+            <v>2.2999999999999998</v>
+          </cell>
+          <cell r="C55">
+            <v>4</v>
+          </cell>
+          <cell r="D55">
+            <v>1.3</v>
+          </cell>
+        </row>
+        <row r="56">
+          <cell r="A56">
+            <v>6.5</v>
+          </cell>
+          <cell r="B56">
+            <v>2.8</v>
+          </cell>
+          <cell r="C56">
+            <v>4.5999999999999996</v>
+          </cell>
+          <cell r="D56">
+            <v>1.5</v>
+          </cell>
+        </row>
+        <row r="57">
+          <cell r="A57">
+            <v>5.7</v>
+          </cell>
+          <cell r="B57">
+            <v>2.8</v>
+          </cell>
+          <cell r="C57">
+            <v>4.5</v>
+          </cell>
+          <cell r="D57">
+            <v>1.3</v>
+          </cell>
+        </row>
+        <row r="58">
+          <cell r="A58">
+            <v>6.3</v>
+          </cell>
+          <cell r="B58">
+            <v>3.3</v>
+          </cell>
+          <cell r="C58">
+            <v>4.7</v>
+          </cell>
+          <cell r="D58">
+            <v>1.6</v>
+          </cell>
+        </row>
+        <row r="59">
+          <cell r="A59">
+            <v>4.9000000000000004</v>
+          </cell>
+          <cell r="B59">
+            <v>2.4</v>
+          </cell>
+          <cell r="C59">
+            <v>3.3</v>
+          </cell>
+          <cell r="D59">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="A60">
+            <v>6.6</v>
+          </cell>
+          <cell r="B60">
+            <v>2.9</v>
+          </cell>
+          <cell r="C60">
+            <v>4.5999999999999996</v>
+          </cell>
+          <cell r="D60">
+            <v>1.3</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="A61">
+            <v>5.2</v>
+          </cell>
+          <cell r="B61">
+            <v>2.7</v>
+          </cell>
+          <cell r="C61">
+            <v>3.9</v>
+          </cell>
+          <cell r="D61">
+            <v>1.4</v>
+          </cell>
+        </row>
+        <row r="62">
+          <cell r="A62">
+            <v>5</v>
+          </cell>
+          <cell r="B62">
+            <v>2</v>
+          </cell>
+          <cell r="C62">
+            <v>3.5</v>
+          </cell>
+          <cell r="D62">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="A63">
+            <v>5.9</v>
+          </cell>
+          <cell r="B63">
+            <v>3</v>
+          </cell>
+          <cell r="C63">
+            <v>4.2</v>
+          </cell>
+          <cell r="D63">
+            <v>1.5</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="A64">
+            <v>6</v>
+          </cell>
+          <cell r="B64">
+            <v>2.2000000000000002</v>
+          </cell>
+          <cell r="C64">
+            <v>4</v>
+          </cell>
+          <cell r="D64">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="A65">
+            <v>6.1</v>
+          </cell>
+          <cell r="B65">
+            <v>2.9</v>
+          </cell>
+          <cell r="C65">
+            <v>4.7</v>
+          </cell>
+          <cell r="D65">
+            <v>1.4</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="A66">
+            <v>5.6</v>
+          </cell>
+          <cell r="B66">
+            <v>2.9</v>
+          </cell>
+          <cell r="C66">
+            <v>3.6</v>
+          </cell>
+          <cell r="D66">
+            <v>1.3</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="A67">
+            <v>6.7</v>
+          </cell>
+          <cell r="B67">
+            <v>3.1</v>
+          </cell>
+          <cell r="C67">
+            <v>4.4000000000000004</v>
+          </cell>
+          <cell r="D67">
+            <v>1.4</v>
+          </cell>
+        </row>
+        <row r="68">
+          <cell r="A68">
+            <v>5.6</v>
+          </cell>
+          <cell r="B68">
+            <v>3</v>
+          </cell>
+          <cell r="C68">
+            <v>4.5</v>
+          </cell>
+          <cell r="D68">
+            <v>1.5</v>
+          </cell>
+        </row>
+        <row r="69">
+          <cell r="A69">
+            <v>5.8</v>
+          </cell>
+          <cell r="B69">
+            <v>2.7</v>
+          </cell>
+          <cell r="C69">
+            <v>4.0999999999999996</v>
+          </cell>
+          <cell r="D69">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="70">
+          <cell r="A70">
+            <v>6.2</v>
+          </cell>
+          <cell r="B70">
+            <v>2.2000000000000002</v>
+          </cell>
+          <cell r="C70">
+            <v>4.5</v>
+          </cell>
+          <cell r="D70">
+            <v>1.5</v>
+          </cell>
+        </row>
+        <row r="71">
+          <cell r="A71">
+            <v>5.6</v>
+          </cell>
+          <cell r="B71">
+            <v>2.5</v>
+          </cell>
+          <cell r="C71">
+            <v>3.9</v>
+          </cell>
+          <cell r="D71">
+            <v>1.1000000000000001</v>
+          </cell>
+        </row>
+        <row r="72">
+          <cell r="A72">
+            <v>5.9</v>
+          </cell>
+          <cell r="B72">
+            <v>3.2</v>
+          </cell>
+          <cell r="C72">
+            <v>4.8</v>
+          </cell>
+          <cell r="D72">
+            <v>1.8</v>
+          </cell>
+        </row>
+        <row r="73">
+          <cell r="A73">
+            <v>6.1</v>
+          </cell>
+          <cell r="B73">
+            <v>2.8</v>
+          </cell>
+          <cell r="C73">
+            <v>4</v>
+          </cell>
+          <cell r="D73">
+            <v>1.3</v>
+          </cell>
+        </row>
+        <row r="74">
+          <cell r="A74">
+            <v>6.3</v>
+          </cell>
+          <cell r="B74">
+            <v>2.5</v>
+          </cell>
+          <cell r="C74">
+            <v>4.9000000000000004</v>
+          </cell>
+          <cell r="D74">
+            <v>1.5</v>
+          </cell>
+        </row>
+        <row r="75">
+          <cell r="A75">
+            <v>6.1</v>
+          </cell>
+          <cell r="B75">
+            <v>2.8</v>
+          </cell>
+          <cell r="C75">
+            <v>4.7</v>
+          </cell>
+          <cell r="D75">
+            <v>1.2</v>
+          </cell>
+        </row>
+        <row r="76">
+          <cell r="A76">
+            <v>6.4</v>
+          </cell>
+          <cell r="B76">
+            <v>2.9</v>
+          </cell>
+          <cell r="C76">
+            <v>4.3</v>
+          </cell>
+          <cell r="D76">
+            <v>1.3</v>
+          </cell>
+        </row>
+        <row r="77">
+          <cell r="A77">
+            <v>6.6</v>
+          </cell>
+          <cell r="B77">
+            <v>3</v>
+          </cell>
+          <cell r="C77">
+            <v>4.4000000000000004</v>
+          </cell>
+          <cell r="D77">
+            <v>1.4</v>
+          </cell>
+        </row>
+        <row r="78">
+          <cell r="A78">
+            <v>6.8</v>
+          </cell>
+          <cell r="B78">
+            <v>2.8</v>
+          </cell>
+          <cell r="C78">
+            <v>4.8</v>
+          </cell>
+          <cell r="D78">
+            <v>1.4</v>
+          </cell>
+        </row>
+        <row r="79">
+          <cell r="A79">
+            <v>6.7</v>
+          </cell>
+          <cell r="B79">
+            <v>3</v>
+          </cell>
+          <cell r="C79">
+            <v>5</v>
+          </cell>
+          <cell r="D79">
+            <v>1.7</v>
+          </cell>
+        </row>
+        <row r="80">
+          <cell r="A80">
+            <v>6</v>
+          </cell>
+          <cell r="B80">
+            <v>2.9</v>
+          </cell>
+          <cell r="C80">
+            <v>4.5</v>
+          </cell>
+          <cell r="D80">
+            <v>1.5</v>
+          </cell>
+        </row>
+        <row r="81">
+          <cell r="A81">
+            <v>5.7</v>
+          </cell>
+          <cell r="B81">
+            <v>2.6</v>
+          </cell>
+          <cell r="C81">
+            <v>3.5</v>
+          </cell>
+          <cell r="D81">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="82">
+          <cell r="A82">
+            <v>5.5</v>
+          </cell>
+          <cell r="B82">
+            <v>2.4</v>
+          </cell>
+          <cell r="C82">
+            <v>3.8</v>
+          </cell>
+          <cell r="D82">
+            <v>1.1000000000000001</v>
+          </cell>
+        </row>
+        <row r="83">
+          <cell r="A83">
+            <v>5.5</v>
+          </cell>
+          <cell r="B83">
+            <v>2.4</v>
+          </cell>
+          <cell r="C83">
+            <v>3.7</v>
+          </cell>
+          <cell r="D83">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="84">
+          <cell r="A84">
+            <v>5.8</v>
+          </cell>
+          <cell r="B84">
+            <v>2.7</v>
+          </cell>
+          <cell r="C84">
+            <v>3.9</v>
+          </cell>
+          <cell r="D84">
+            <v>1.2</v>
+          </cell>
+        </row>
+        <row r="85">
+          <cell r="A85">
+            <v>6</v>
+          </cell>
+          <cell r="B85">
+            <v>2.7</v>
+          </cell>
+          <cell r="C85">
+            <v>5.0999999999999996</v>
+          </cell>
+          <cell r="D85">
+            <v>1.6</v>
+          </cell>
+        </row>
+        <row r="86">
+          <cell r="A86">
+            <v>5.4</v>
+          </cell>
+          <cell r="B86">
+            <v>3</v>
+          </cell>
+          <cell r="C86">
+            <v>4.5</v>
+          </cell>
+          <cell r="D86">
+            <v>1.5</v>
+          </cell>
+        </row>
+        <row r="87">
+          <cell r="A87">
+            <v>6</v>
+          </cell>
+          <cell r="B87">
+            <v>3.4</v>
+          </cell>
+          <cell r="C87">
+            <v>4.5</v>
+          </cell>
+          <cell r="D87">
+            <v>1.6</v>
+          </cell>
+        </row>
+        <row r="88">
+          <cell r="A88">
+            <v>6.7</v>
+          </cell>
+          <cell r="B88">
+            <v>3.1</v>
+          </cell>
+          <cell r="C88">
+            <v>4.7</v>
+          </cell>
+          <cell r="D88">
+            <v>1.5</v>
+          </cell>
+        </row>
+        <row r="89">
+          <cell r="A89">
+            <v>6.3</v>
+          </cell>
+          <cell r="B89">
+            <v>2.2999999999999998</v>
+          </cell>
+          <cell r="C89">
+            <v>4.4000000000000004</v>
+          </cell>
+          <cell r="D89">
+            <v>1.3</v>
+          </cell>
+        </row>
+        <row r="90">
+          <cell r="A90">
+            <v>5.6</v>
+          </cell>
+          <cell r="B90">
+            <v>3</v>
+          </cell>
+          <cell r="C90">
+            <v>4.0999999999999996</v>
+          </cell>
+          <cell r="D90">
+            <v>1.3</v>
+          </cell>
+        </row>
+        <row r="91">
+          <cell r="A91">
+            <v>5.5</v>
+          </cell>
+          <cell r="B91">
+            <v>2.5</v>
+          </cell>
+          <cell r="C91">
+            <v>4</v>
+          </cell>
+          <cell r="D91">
+            <v>1.3</v>
+          </cell>
+        </row>
+        <row r="92">
+          <cell r="A92">
+            <v>5.5</v>
+          </cell>
+          <cell r="B92">
+            <v>2.6</v>
+          </cell>
+          <cell r="C92">
+            <v>4.4000000000000004</v>
+          </cell>
+          <cell r="D92">
+            <v>1.2</v>
+          </cell>
+        </row>
+        <row r="93">
+          <cell r="A93">
+            <v>6.1</v>
+          </cell>
+          <cell r="B93">
+            <v>3</v>
+          </cell>
+          <cell r="C93">
+            <v>4.5999999999999996</v>
+          </cell>
+          <cell r="D93">
+            <v>1.4</v>
+          </cell>
+        </row>
+        <row r="94">
+          <cell r="A94">
+            <v>5.8</v>
+          </cell>
+          <cell r="B94">
+            <v>2.6</v>
+          </cell>
+          <cell r="C94">
+            <v>4</v>
+          </cell>
+          <cell r="D94">
+            <v>1.2</v>
+          </cell>
+        </row>
+        <row r="95">
+          <cell r="A95">
+            <v>5</v>
+          </cell>
+          <cell r="B95">
+            <v>2.2999999999999998</v>
+          </cell>
+          <cell r="C95">
+            <v>3.3</v>
+          </cell>
+          <cell r="D95">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="96">
+          <cell r="A96">
+            <v>5.6</v>
+          </cell>
+          <cell r="B96">
+            <v>2.7</v>
+          </cell>
+          <cell r="C96">
+            <v>4.2</v>
+          </cell>
+          <cell r="D96">
+            <v>1.3</v>
+          </cell>
+        </row>
+        <row r="97">
+          <cell r="A97">
+            <v>5.7</v>
+          </cell>
+          <cell r="B97">
+            <v>3</v>
+          </cell>
+          <cell r="C97">
+            <v>4.2</v>
+          </cell>
+          <cell r="D97">
+            <v>1.2</v>
+          </cell>
+        </row>
+        <row r="98">
+          <cell r="A98">
+            <v>5.7</v>
+          </cell>
+          <cell r="B98">
+            <v>2.9</v>
+          </cell>
+          <cell r="C98">
+            <v>4.2</v>
+          </cell>
+          <cell r="D98">
+            <v>1.3</v>
+          </cell>
+        </row>
+        <row r="99">
+          <cell r="A99">
+            <v>6.2</v>
+          </cell>
+          <cell r="B99">
+            <v>2.9</v>
+          </cell>
+          <cell r="C99">
+            <v>4.3</v>
+          </cell>
+          <cell r="D99">
+            <v>1.3</v>
+          </cell>
+        </row>
+        <row r="100">
+          <cell r="A100">
+            <v>5.0999999999999996</v>
+          </cell>
+          <cell r="B100">
+            <v>2.5</v>
+          </cell>
+          <cell r="C100">
+            <v>3</v>
+          </cell>
+          <cell r="D100">
+            <v>1.1000000000000001</v>
+          </cell>
+        </row>
+        <row r="101">
+          <cell r="A101">
+            <v>5.7</v>
+          </cell>
+          <cell r="B101">
+            <v>2.8</v>
+          </cell>
+          <cell r="C101">
+            <v>4.0999999999999996</v>
+          </cell>
+          <cell r="D101">
+            <v>1.3</v>
+          </cell>
+        </row>
+        <row r="102">
+          <cell r="A102">
+            <v>6.3</v>
+          </cell>
+          <cell r="B102">
+            <v>3.3</v>
+          </cell>
+          <cell r="C102">
+            <v>6</v>
+          </cell>
+          <cell r="D102">
+            <v>2.5</v>
+          </cell>
+          <cell r="E102" t="str">
+            <v>iris_virginica</v>
+          </cell>
+        </row>
+        <row r="103">
+          <cell r="A103">
+            <v>5.8</v>
+          </cell>
+          <cell r="B103">
+            <v>2.7</v>
+          </cell>
+          <cell r="C103">
+            <v>5.0999999999999996</v>
+          </cell>
+          <cell r="D103">
+            <v>1.9</v>
+          </cell>
+        </row>
+        <row r="104">
+          <cell r="A104">
+            <v>7.1</v>
+          </cell>
+          <cell r="B104">
+            <v>3</v>
+          </cell>
+          <cell r="C104">
+            <v>5.9</v>
+          </cell>
+          <cell r="D104">
+            <v>2.1</v>
+          </cell>
+        </row>
+        <row r="105">
+          <cell r="A105">
+            <v>6.3</v>
+          </cell>
+          <cell r="B105">
+            <v>2.9</v>
+          </cell>
+          <cell r="C105">
+            <v>5.6</v>
+          </cell>
+          <cell r="D105">
+            <v>1.8</v>
+          </cell>
+        </row>
+        <row r="106">
+          <cell r="A106">
+            <v>6.5</v>
+          </cell>
+          <cell r="B106">
+            <v>3</v>
+          </cell>
+          <cell r="C106">
+            <v>5.8</v>
+          </cell>
+          <cell r="D106">
+            <v>2.2000000000000002</v>
+          </cell>
+        </row>
+        <row r="107">
+          <cell r="A107">
+            <v>7.6</v>
+          </cell>
+          <cell r="B107">
+            <v>3</v>
+          </cell>
+          <cell r="C107">
+            <v>6.6</v>
+          </cell>
+          <cell r="D107">
+            <v>2.1</v>
+          </cell>
+        </row>
+        <row r="108">
+          <cell r="A108">
+            <v>4.9000000000000004</v>
+          </cell>
+          <cell r="B108">
+            <v>2.5</v>
+          </cell>
+          <cell r="C108">
+            <v>4.5</v>
+          </cell>
+          <cell r="D108">
+            <v>1.7</v>
+          </cell>
+        </row>
+        <row r="109">
+          <cell r="A109">
+            <v>7.3</v>
+          </cell>
+          <cell r="B109">
+            <v>2.9</v>
+          </cell>
+          <cell r="C109">
+            <v>6.3</v>
+          </cell>
+          <cell r="D109">
+            <v>1.8</v>
+          </cell>
+        </row>
+        <row r="110">
+          <cell r="A110">
+            <v>6.7</v>
+          </cell>
+          <cell r="B110">
+            <v>2.5</v>
+          </cell>
+          <cell r="C110">
+            <v>5.8</v>
+          </cell>
+          <cell r="D110">
+            <v>1.8</v>
+          </cell>
+        </row>
+        <row r="111">
+          <cell r="A111">
+            <v>7.2</v>
+          </cell>
+          <cell r="B111">
+            <v>3.6</v>
+          </cell>
+          <cell r="C111">
+            <v>6.1</v>
+          </cell>
+          <cell r="D111">
+            <v>2.5</v>
+          </cell>
+        </row>
+        <row r="112">
+          <cell r="A112">
+            <v>6.5</v>
+          </cell>
+          <cell r="B112">
+            <v>3.2</v>
+          </cell>
+          <cell r="C112">
+            <v>5.0999999999999996</v>
+          </cell>
+          <cell r="D112">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="113">
+          <cell r="A113">
+            <v>6.4</v>
+          </cell>
+          <cell r="B113">
+            <v>2.7</v>
+          </cell>
+          <cell r="C113">
+            <v>5.3</v>
+          </cell>
+          <cell r="D113">
+            <v>1.9</v>
+          </cell>
+        </row>
+        <row r="114">
+          <cell r="A114">
+            <v>6.8</v>
+          </cell>
+          <cell r="B114">
+            <v>3</v>
+          </cell>
+          <cell r="C114">
+            <v>5.5</v>
+          </cell>
+          <cell r="D114">
+            <v>2.1</v>
+          </cell>
+        </row>
+        <row r="115">
+          <cell r="A115">
+            <v>5.7</v>
+          </cell>
+          <cell r="B115">
+            <v>2.5</v>
+          </cell>
+          <cell r="C115">
+            <v>5</v>
+          </cell>
+          <cell r="D115">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="116">
+          <cell r="A116">
+            <v>5.8</v>
+          </cell>
+          <cell r="B116">
+            <v>2.8</v>
+          </cell>
+          <cell r="C116">
+            <v>5.0999999999999996</v>
+          </cell>
+          <cell r="D116">
+            <v>2.4</v>
+          </cell>
+        </row>
+        <row r="117">
+          <cell r="A117">
+            <v>6.4</v>
+          </cell>
+          <cell r="B117">
+            <v>3.2</v>
+          </cell>
+          <cell r="C117">
+            <v>5.3</v>
+          </cell>
+          <cell r="D117">
+            <v>2.2999999999999998</v>
+          </cell>
+        </row>
+        <row r="118">
+          <cell r="A118">
+            <v>6.5</v>
+          </cell>
+          <cell r="B118">
+            <v>3</v>
+          </cell>
+          <cell r="C118">
+            <v>5.5</v>
+          </cell>
+          <cell r="D118">
+            <v>1.8</v>
+          </cell>
+        </row>
+        <row r="119">
+          <cell r="A119">
+            <v>7.7</v>
+          </cell>
+          <cell r="B119">
+            <v>3.8</v>
+          </cell>
+          <cell r="C119">
+            <v>6.7</v>
+          </cell>
+          <cell r="D119">
+            <v>2.2000000000000002</v>
+          </cell>
+        </row>
+        <row r="120">
+          <cell r="A120">
+            <v>7.7</v>
+          </cell>
+          <cell r="B120">
+            <v>2.6</v>
+          </cell>
+          <cell r="C120">
+            <v>6.9</v>
+          </cell>
+          <cell r="D120">
+            <v>2.2999999999999998</v>
+          </cell>
+        </row>
+        <row r="121">
+          <cell r="A121">
+            <v>6</v>
+          </cell>
+          <cell r="B121">
+            <v>2.2000000000000002</v>
+          </cell>
+          <cell r="C121">
+            <v>5</v>
+          </cell>
+          <cell r="D121">
+            <v>1.5</v>
+          </cell>
+        </row>
+        <row r="122">
+          <cell r="A122">
+            <v>6.9</v>
+          </cell>
+          <cell r="B122">
+            <v>3.2</v>
+          </cell>
+          <cell r="C122">
+            <v>5.7</v>
+          </cell>
+          <cell r="D122">
+            <v>2.2999999999999998</v>
+          </cell>
+        </row>
+        <row r="123">
+          <cell r="A123">
+            <v>5.6</v>
+          </cell>
+          <cell r="B123">
+            <v>2.8</v>
+          </cell>
+          <cell r="C123">
+            <v>4.9000000000000004</v>
+          </cell>
+          <cell r="D123">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="124">
+          <cell r="A124">
+            <v>7.7</v>
+          </cell>
+          <cell r="B124">
+            <v>2.8</v>
+          </cell>
+          <cell r="C124">
+            <v>6.7</v>
+          </cell>
+          <cell r="D124">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="125">
+          <cell r="A125">
+            <v>6.3</v>
+          </cell>
+          <cell r="B125">
+            <v>2.7</v>
+          </cell>
+          <cell r="C125">
+            <v>4.9000000000000004</v>
+          </cell>
+          <cell r="D125">
+            <v>1.8</v>
+          </cell>
+        </row>
+        <row r="126">
+          <cell r="A126">
+            <v>6.7</v>
+          </cell>
+          <cell r="B126">
+            <v>3.3</v>
+          </cell>
+          <cell r="C126">
+            <v>5.7</v>
+          </cell>
+          <cell r="D126">
+            <v>2.1</v>
+          </cell>
+        </row>
+        <row r="127">
+          <cell r="A127">
+            <v>7.2</v>
+          </cell>
+          <cell r="B127">
+            <v>3.2</v>
+          </cell>
+          <cell r="C127">
+            <v>6</v>
+          </cell>
+          <cell r="D127">
+            <v>1.8</v>
+          </cell>
+        </row>
+        <row r="128">
+          <cell r="A128">
+            <v>6.2</v>
+          </cell>
+          <cell r="B128">
+            <v>2.8</v>
+          </cell>
+          <cell r="C128">
+            <v>4.8</v>
+          </cell>
+          <cell r="D128">
+            <v>1.8</v>
+          </cell>
+        </row>
+        <row r="129">
+          <cell r="A129">
+            <v>6.1</v>
+          </cell>
+          <cell r="B129">
+            <v>3</v>
+          </cell>
+          <cell r="C129">
+            <v>4.9000000000000004</v>
+          </cell>
+          <cell r="D129">
+            <v>1.8</v>
+          </cell>
+        </row>
+        <row r="130">
+          <cell r="A130">
+            <v>6.4</v>
+          </cell>
+          <cell r="B130">
+            <v>2.8</v>
+          </cell>
+          <cell r="C130">
+            <v>5.6</v>
+          </cell>
+          <cell r="D130">
+            <v>2.1</v>
+          </cell>
+        </row>
+        <row r="131">
+          <cell r="A131">
+            <v>7.2</v>
+          </cell>
+          <cell r="B131">
+            <v>3</v>
+          </cell>
+          <cell r="C131">
+            <v>5.8</v>
+          </cell>
+          <cell r="D131">
+            <v>1.6</v>
+          </cell>
+        </row>
+        <row r="132">
+          <cell r="A132">
+            <v>7.4</v>
+          </cell>
+          <cell r="B132">
+            <v>2.8</v>
+          </cell>
+          <cell r="C132">
+            <v>6.1</v>
+          </cell>
+          <cell r="D132">
+            <v>1.9</v>
+          </cell>
+        </row>
+        <row r="133">
+          <cell r="A133">
+            <v>7.9</v>
+          </cell>
+          <cell r="B133">
+            <v>3.8</v>
+          </cell>
+          <cell r="C133">
+            <v>6.4</v>
+          </cell>
+          <cell r="D133">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="134">
+          <cell r="A134">
+            <v>6.4</v>
+          </cell>
+          <cell r="B134">
+            <v>2.8</v>
+          </cell>
+          <cell r="C134">
+            <v>5.6</v>
+          </cell>
+          <cell r="D134">
+            <v>2.2000000000000002</v>
+          </cell>
+        </row>
+        <row r="135">
+          <cell r="A135">
+            <v>6.3</v>
+          </cell>
+          <cell r="B135">
+            <v>2.8</v>
+          </cell>
+          <cell r="C135">
+            <v>5.0999999999999996</v>
+          </cell>
+          <cell r="D135">
+            <v>1.5</v>
+          </cell>
+        </row>
+        <row r="136">
+          <cell r="A136">
+            <v>6.1</v>
+          </cell>
+          <cell r="B136">
+            <v>2.6</v>
+          </cell>
+          <cell r="C136">
+            <v>5.6</v>
+          </cell>
+          <cell r="D136">
+            <v>1.4</v>
+          </cell>
+        </row>
+        <row r="137">
+          <cell r="A137">
+            <v>7.7</v>
+          </cell>
+          <cell r="B137">
+            <v>3</v>
+          </cell>
+          <cell r="C137">
+            <v>6.1</v>
+          </cell>
+          <cell r="D137">
+            <v>2.2999999999999998</v>
+          </cell>
+        </row>
+        <row r="138">
+          <cell r="A138">
+            <v>6.3</v>
+          </cell>
+          <cell r="B138">
+            <v>3.4</v>
+          </cell>
+          <cell r="C138">
+            <v>5.6</v>
+          </cell>
+          <cell r="D138">
+            <v>2.4</v>
+          </cell>
+        </row>
+        <row r="139">
+          <cell r="A139">
+            <v>6.4</v>
+          </cell>
+          <cell r="B139">
+            <v>3.1</v>
+          </cell>
+          <cell r="C139">
+            <v>5.5</v>
+          </cell>
+          <cell r="D139">
+            <v>1.8</v>
+          </cell>
+        </row>
+        <row r="140">
+          <cell r="A140">
+            <v>6</v>
+          </cell>
+          <cell r="B140">
+            <v>3</v>
+          </cell>
+          <cell r="C140">
+            <v>4.8</v>
+          </cell>
+          <cell r="D140">
+            <v>1.8</v>
+          </cell>
+        </row>
+        <row r="141">
+          <cell r="A141">
+            <v>6.9</v>
+          </cell>
+          <cell r="B141">
+            <v>3.1</v>
+          </cell>
+          <cell r="C141">
+            <v>5.4</v>
+          </cell>
+          <cell r="D141">
+            <v>2.1</v>
+          </cell>
+        </row>
+        <row r="142">
+          <cell r="A142">
+            <v>6.7</v>
+          </cell>
+          <cell r="B142">
+            <v>3.1</v>
+          </cell>
+          <cell r="C142">
+            <v>5.6</v>
+          </cell>
+          <cell r="D142">
+            <v>2.4</v>
+          </cell>
+        </row>
+        <row r="143">
+          <cell r="A143">
+            <v>6.9</v>
+          </cell>
+          <cell r="B143">
+            <v>3.1</v>
+          </cell>
+          <cell r="C143">
+            <v>5.0999999999999996</v>
+          </cell>
+          <cell r="D143">
+            <v>2.2999999999999998</v>
+          </cell>
+        </row>
+        <row r="144">
+          <cell r="A144">
+            <v>5.8</v>
+          </cell>
+          <cell r="B144">
+            <v>2.7</v>
+          </cell>
+          <cell r="C144">
+            <v>5.0999999999999996</v>
+          </cell>
+          <cell r="D144">
+            <v>1.9</v>
+          </cell>
+        </row>
+        <row r="145">
+          <cell r="A145">
+            <v>6.8</v>
+          </cell>
+          <cell r="B145">
+            <v>3.2</v>
+          </cell>
+          <cell r="C145">
+            <v>5.9</v>
+          </cell>
+          <cell r="D145">
+            <v>2.2999999999999998</v>
+          </cell>
+        </row>
+        <row r="146">
+          <cell r="A146">
+            <v>6.7</v>
+          </cell>
+          <cell r="B146">
+            <v>3.3</v>
+          </cell>
+          <cell r="C146">
+            <v>5.7</v>
+          </cell>
+          <cell r="D146">
+            <v>2.5</v>
+          </cell>
+        </row>
+        <row r="147">
+          <cell r="A147">
+            <v>6.7</v>
+          </cell>
+          <cell r="B147">
+            <v>3</v>
+          </cell>
+          <cell r="C147">
+            <v>5.2</v>
+          </cell>
+          <cell r="D147">
+            <v>2.2999999999999998</v>
+          </cell>
+        </row>
+        <row r="148">
+          <cell r="A148">
+            <v>6.3</v>
+          </cell>
+          <cell r="B148">
+            <v>2.5</v>
+          </cell>
+          <cell r="C148">
+            <v>5</v>
+          </cell>
+          <cell r="D148">
+            <v>1.9</v>
+          </cell>
+        </row>
+        <row r="149">
+          <cell r="A149">
+            <v>6.5</v>
+          </cell>
+          <cell r="B149">
+            <v>3</v>
+          </cell>
+          <cell r="C149">
+            <v>5.2</v>
+          </cell>
+          <cell r="D149">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="150">
+          <cell r="A150">
+            <v>6.2</v>
+          </cell>
+          <cell r="B150">
+            <v>3.4</v>
+          </cell>
+          <cell r="C150">
+            <v>5.4</v>
+          </cell>
+          <cell r="D150">
+            <v>2.2999999999999998</v>
+          </cell>
+        </row>
+        <row r="151">
+          <cell r="A151">
+            <v>5.9</v>
+          </cell>
+          <cell r="B151">
+            <v>3</v>
+          </cell>
+          <cell r="C151">
+            <v>5.0999999999999996</v>
+          </cell>
+          <cell r="D151">
+            <v>1.8</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -16198,7 +18324,7 @@
   <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Fixed adaptive learning and early stopping
</commit_message>
<xml_diff>
--- a/test/YANNL-walkthrough.xlsx
+++ b/test/YANNL-walkthrough.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MDeloison\_Never Backup\Cpp\YANNL-vc\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BAD3799-FA42-461B-9A17-83B60CF0AB26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE2F2F1-62B9-48AD-8AA9-7727D346F7E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="5" xr2:uid="{3DE57AAC-3496-42F8-B681-7BA2B7FE7A12}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="9" xr2:uid="{3DE57AAC-3496-42F8-B681-7BA2B7FE7A12}"/>
   </bookViews>
   <sheets>
     <sheet name="No bias" sheetId="1" r:id="rId1"/>
@@ -22,11 +22,9 @@
     <sheet name="Momentum" sheetId="9" r:id="rId7"/>
     <sheet name="Softmax 2 outputs" sheetId="11" r:id="rId8"/>
     <sheet name="Softmax 3 outputs" sheetId="13" r:id="rId9"/>
-    <sheet name="Class structure" sheetId="12" r:id="rId10"/>
+    <sheet name="Batches" sheetId="15" r:id="rId10"/>
+    <sheet name="Class structure" sheetId="12" r:id="rId11"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId11"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -46,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="108">
   <si>
     <t>i1</t>
   </si>
@@ -525,6 +523,24 @@
   <si>
     <t>droppedNeuron</t>
   </si>
+  <si>
+    <t>calcError/Mean Squared Error</t>
+  </si>
+  <si>
+    <t>calcError/Cross Entropy Error</t>
+  </si>
+  <si>
+    <t>saveToFile (override)</t>
+  </si>
+  <si>
+    <t>saveToFile (no type)</t>
+  </si>
+  <si>
+    <t>Forward pass and error #1</t>
+  </si>
+  <si>
+    <t>Forward pass and error #2</t>
+  </si>
 </sst>
 </file>
 
@@ -669,7 +685,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -762,6 +778,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2098,6 +2117,1919 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Straight Arrow Connector 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3CBBD93-E60D-455E-BD95-B2A783538C38}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1889760" y="975360"/>
+          <a:ext cx="1752600" cy="7620"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A0A14F5-ED80-4051-BFD1-FA61F1B6FF59}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1905000" y="1066800"/>
+          <a:ext cx="1661160" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5478E16-B5CA-46F4-90A2-EA29343457D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1889760" y="1066800"/>
+          <a:ext cx="1737360" cy="792480"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>525780</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07E26955-47B8-4275-BD03-06A650734D6C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1866900" y="1943100"/>
+          <a:ext cx="1706880" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>541020</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1A8919A-883E-4A3E-9191-94310912232D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1874520" y="1127760"/>
+          <a:ext cx="1714500" cy="1844040"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53EBEF2B-F325-4B14-9304-C6DDCCBD0804}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1920240" y="2133600"/>
+          <a:ext cx="1684020" cy="853440"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9877A259-DD93-4696-A596-AA20AD23DF59}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4937760" y="975360"/>
+          <a:ext cx="1752600" cy="7620"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B5BCF78-9277-4ECA-A603-4916855DA65D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4953000" y="1066800"/>
+          <a:ext cx="1661160" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Arrow Connector 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BD6F6F7-C743-414F-A2C5-30E93DF50BD0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4937760" y="1066800"/>
+          <a:ext cx="1737360" cy="792480"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>525780</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EB0E51F-EFFD-4355-89D4-9B1BE267A1C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4914900" y="1943100"/>
+          <a:ext cx="1706880" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>541020</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Straight Arrow Connector 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A180B49D-D7A8-4DC2-87AA-13A62093C2AC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4922520" y="1127760"/>
+          <a:ext cx="1714500" cy="1844040"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65F6C488-ED03-46C4-A4A5-FFFC7235EAA9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4968240" y="2133600"/>
+          <a:ext cx="1684020" cy="853440"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51294F99-4A1D-461E-94E2-2BA35431ADC7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1889760" y="4450080"/>
+          <a:ext cx="1752600" cy="7620"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97F1A994-5EE7-4D5A-BCD4-6E06FDFF1C73}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1905000" y="4541520"/>
+          <a:ext cx="1661160" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1003256B-2AB5-472B-9D9A-E0A4F1838C29}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1889760" y="4541520"/>
+          <a:ext cx="1737360" cy="792480"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>525780</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Straight Arrow Connector 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89ECB395-8AA3-4674-A6A3-A2B6D7258027}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1866900" y="5417820"/>
+          <a:ext cx="1706880" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>541020</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Straight Arrow Connector 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{397D3615-5F97-4A58-BC21-0C36B5AFCA65}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1874520" y="4602480"/>
+          <a:ext cx="1714500" cy="1844040"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Arrow Connector 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{814BB24B-98A1-4536-8DF7-783DFC9A2354}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1920240" y="5608320"/>
+          <a:ext cx="1684020" cy="853440"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Straight Arrow Connector 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02F54051-45CF-4934-9CA5-1B5769B3D0F6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4937760" y="4450080"/>
+          <a:ext cx="1752600" cy="7620"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Straight Arrow Connector 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3441E51-381A-4886-83AA-B57C68F41423}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4953000" y="4541520"/>
+          <a:ext cx="1661160" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Straight Arrow Connector 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{964BC684-EBCF-4156-85E0-E69DF702109D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4937760" y="4541520"/>
+          <a:ext cx="1737360" cy="792480"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>525780</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Straight Arrow Connector 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1B1D180-320F-4B63-A9EC-4059596AB69B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4914900" y="5417820"/>
+          <a:ext cx="1706880" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>541020</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12C3A7CC-1292-4C85-A546-4813933AF7E2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4922520" y="4602480"/>
+          <a:ext cx="1714500" cy="1844040"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Straight Arrow Connector 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2846C11-0BDE-486F-AB5F-658811BE4402}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4968240" y="5608320"/>
+          <a:ext cx="1684020" cy="853440"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Straight Arrow Connector 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDE76726-E308-4D39-83C0-EAE0A99DFCC5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1889760" y="986246"/>
+          <a:ext cx="1752600" cy="7620"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="Straight Arrow Connector 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39C74A0E-C509-4092-B53D-42D91A6F74B0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1905000" y="1077686"/>
+          <a:ext cx="1661160" cy="772885"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="Straight Arrow Connector 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B1CEFF5-B84A-42F9-A7E1-0E4D2634D853}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1889760" y="1077686"/>
+          <a:ext cx="1737360" cy="803365"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>525780</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="Straight Arrow Connector 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAA36A7C-7E5E-4D63-8E3A-40C4A58778EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1866900" y="1964871"/>
+          <a:ext cx="1706880" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>541020</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="Straight Arrow Connector 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDF9B38D-F96B-4B55-B028-9E1F73F77A86}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1874520" y="1140823"/>
+          <a:ext cx="1714500" cy="1865811"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="Straight Arrow Connector 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10994448-136C-43FF-AA86-91C942850B46}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1920240" y="2157549"/>
+          <a:ext cx="1684020" cy="864325"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="32" name="Straight Arrow Connector 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91ACD90E-1EA5-4488-AC70-8768C3D7E424}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4937760" y="986246"/>
+          <a:ext cx="1752600" cy="7620"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="Straight Arrow Connector 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9639BFF3-65CC-40F8-ADFC-3C786F829679}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4953000" y="1077686"/>
+          <a:ext cx="1661160" cy="772885"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="Straight Arrow Connector 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{06E5FBFF-E566-4686-B841-36A1B409CD80}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4937760" y="1077686"/>
+          <a:ext cx="1737360" cy="803365"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>525780</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="35" name="Straight Arrow Connector 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC315791-2311-44E1-A3D6-B4D35DCAC198}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4914900" y="1964871"/>
+          <a:ext cx="1706880" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>541020</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="Straight Arrow Connector 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFD0669F-356E-4A7A-8B49-F8AE978C870F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4922520" y="1140823"/>
+          <a:ext cx="1714500" cy="1865811"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="Straight Arrow Connector 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93A266DE-07A1-4D45-82EB-2F2A7C7BF45E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4968240" y="2157549"/>
+          <a:ext cx="1684020" cy="864325"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -15451,2129 +17383,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="A2">
-            <v>5.0999999999999996</v>
-          </cell>
-          <cell r="B2">
-            <v>3.5</v>
-          </cell>
-          <cell r="C2">
-            <v>1.4</v>
-          </cell>
-          <cell r="D2">
-            <v>0.2</v>
-          </cell>
-          <cell r="E2" t="str">
-            <v>iris_setosa</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3">
-            <v>4.9000000000000004</v>
-          </cell>
-          <cell r="B3">
-            <v>3</v>
-          </cell>
-          <cell r="C3">
-            <v>1.4</v>
-          </cell>
-          <cell r="D3">
-            <v>0.2</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4">
-            <v>4.7</v>
-          </cell>
-          <cell r="B4">
-            <v>3.2</v>
-          </cell>
-          <cell r="C4">
-            <v>1.3</v>
-          </cell>
-          <cell r="D4">
-            <v>0.2</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5">
-            <v>4.5999999999999996</v>
-          </cell>
-          <cell r="B5">
-            <v>3.1</v>
-          </cell>
-          <cell r="C5">
-            <v>1.5</v>
-          </cell>
-          <cell r="D5">
-            <v>0.2</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6">
-            <v>5</v>
-          </cell>
-          <cell r="B6">
-            <v>3.6</v>
-          </cell>
-          <cell r="C6">
-            <v>1.4</v>
-          </cell>
-          <cell r="D6">
-            <v>0.2</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7">
-            <v>5.4</v>
-          </cell>
-          <cell r="B7">
-            <v>3.9</v>
-          </cell>
-          <cell r="C7">
-            <v>1.7</v>
-          </cell>
-          <cell r="D7">
-            <v>0.4</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8">
-            <v>4.5999999999999996</v>
-          </cell>
-          <cell r="B8">
-            <v>3.4</v>
-          </cell>
-          <cell r="C8">
-            <v>1.4</v>
-          </cell>
-          <cell r="D8">
-            <v>0.3</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9">
-            <v>5</v>
-          </cell>
-          <cell r="B9">
-            <v>3.4</v>
-          </cell>
-          <cell r="C9">
-            <v>1.5</v>
-          </cell>
-          <cell r="D9">
-            <v>0.2</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10">
-            <v>4.4000000000000004</v>
-          </cell>
-          <cell r="B10">
-            <v>2.9</v>
-          </cell>
-          <cell r="C10">
-            <v>1.4</v>
-          </cell>
-          <cell r="D10">
-            <v>0.2</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11">
-            <v>4.9000000000000004</v>
-          </cell>
-          <cell r="B11">
-            <v>3.1</v>
-          </cell>
-          <cell r="C11">
-            <v>1.5</v>
-          </cell>
-          <cell r="D11">
-            <v>0.1</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12">
-            <v>5.4</v>
-          </cell>
-          <cell r="B12">
-            <v>3.7</v>
-          </cell>
-          <cell r="C12">
-            <v>1.5</v>
-          </cell>
-          <cell r="D12">
-            <v>0.2</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13">
-            <v>4.8</v>
-          </cell>
-          <cell r="B13">
-            <v>3.4</v>
-          </cell>
-          <cell r="C13">
-            <v>1.6</v>
-          </cell>
-          <cell r="D13">
-            <v>0.2</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14">
-            <v>4.8</v>
-          </cell>
-          <cell r="B14">
-            <v>3</v>
-          </cell>
-          <cell r="C14">
-            <v>1.4</v>
-          </cell>
-          <cell r="D14">
-            <v>0.1</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15">
-            <v>4.3</v>
-          </cell>
-          <cell r="B15">
-            <v>3</v>
-          </cell>
-          <cell r="C15">
-            <v>1.1000000000000001</v>
-          </cell>
-          <cell r="D15">
-            <v>0.1</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16">
-            <v>5.8</v>
-          </cell>
-          <cell r="B16">
-            <v>4</v>
-          </cell>
-          <cell r="C16">
-            <v>1.2</v>
-          </cell>
-          <cell r="D16">
-            <v>0.2</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17">
-            <v>5.7</v>
-          </cell>
-          <cell r="B17">
-            <v>4.4000000000000004</v>
-          </cell>
-          <cell r="C17">
-            <v>1.5</v>
-          </cell>
-          <cell r="D17">
-            <v>0.4</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18">
-            <v>5.4</v>
-          </cell>
-          <cell r="B18">
-            <v>3.9</v>
-          </cell>
-          <cell r="C18">
-            <v>1.3</v>
-          </cell>
-          <cell r="D18">
-            <v>0.4</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="A19">
-            <v>5.0999999999999996</v>
-          </cell>
-          <cell r="B19">
-            <v>3.5</v>
-          </cell>
-          <cell r="C19">
-            <v>1.4</v>
-          </cell>
-          <cell r="D19">
-            <v>0.3</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="A20">
-            <v>5.7</v>
-          </cell>
-          <cell r="B20">
-            <v>3.8</v>
-          </cell>
-          <cell r="C20">
-            <v>1.7</v>
-          </cell>
-          <cell r="D20">
-            <v>0.3</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="A21">
-            <v>5.0999999999999996</v>
-          </cell>
-          <cell r="B21">
-            <v>3.8</v>
-          </cell>
-          <cell r="C21">
-            <v>1.5</v>
-          </cell>
-          <cell r="D21">
-            <v>0.3</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="A22">
-            <v>5.4</v>
-          </cell>
-          <cell r="B22">
-            <v>3.4</v>
-          </cell>
-          <cell r="C22">
-            <v>1.7</v>
-          </cell>
-          <cell r="D22">
-            <v>0.2</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="A23">
-            <v>5.0999999999999996</v>
-          </cell>
-          <cell r="B23">
-            <v>3.7</v>
-          </cell>
-          <cell r="C23">
-            <v>1.5</v>
-          </cell>
-          <cell r="D23">
-            <v>0.4</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="A24">
-            <v>4.5999999999999996</v>
-          </cell>
-          <cell r="B24">
-            <v>3.6</v>
-          </cell>
-          <cell r="C24">
-            <v>1</v>
-          </cell>
-          <cell r="D24">
-            <v>0.2</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="A25">
-            <v>5.0999999999999996</v>
-          </cell>
-          <cell r="B25">
-            <v>3.3</v>
-          </cell>
-          <cell r="C25">
-            <v>1.7</v>
-          </cell>
-          <cell r="D25">
-            <v>0.5</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="A26">
-            <v>4.8</v>
-          </cell>
-          <cell r="B26">
-            <v>3.4</v>
-          </cell>
-          <cell r="C26">
-            <v>1.9</v>
-          </cell>
-          <cell r="D26">
-            <v>0.2</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="A27">
-            <v>5</v>
-          </cell>
-          <cell r="B27">
-            <v>3</v>
-          </cell>
-          <cell r="C27">
-            <v>1.6</v>
-          </cell>
-          <cell r="D27">
-            <v>0.2</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="A28">
-            <v>5</v>
-          </cell>
-          <cell r="B28">
-            <v>3.4</v>
-          </cell>
-          <cell r="C28">
-            <v>1.6</v>
-          </cell>
-          <cell r="D28">
-            <v>0.4</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="A29">
-            <v>5.2</v>
-          </cell>
-          <cell r="B29">
-            <v>3.5</v>
-          </cell>
-          <cell r="C29">
-            <v>1.5</v>
-          </cell>
-          <cell r="D29">
-            <v>0.2</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="A30">
-            <v>5.2</v>
-          </cell>
-          <cell r="B30">
-            <v>3.4</v>
-          </cell>
-          <cell r="C30">
-            <v>1.4</v>
-          </cell>
-          <cell r="D30">
-            <v>0.2</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="A31">
-            <v>4.7</v>
-          </cell>
-          <cell r="B31">
-            <v>3.2</v>
-          </cell>
-          <cell r="C31">
-            <v>1.6</v>
-          </cell>
-          <cell r="D31">
-            <v>0.2</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="A32">
-            <v>4.8</v>
-          </cell>
-          <cell r="B32">
-            <v>3.1</v>
-          </cell>
-          <cell r="C32">
-            <v>1.6</v>
-          </cell>
-          <cell r="D32">
-            <v>0.2</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="A33">
-            <v>5.4</v>
-          </cell>
-          <cell r="B33">
-            <v>3.4</v>
-          </cell>
-          <cell r="C33">
-            <v>1.5</v>
-          </cell>
-          <cell r="D33">
-            <v>0.4</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="A34">
-            <v>5.2</v>
-          </cell>
-          <cell r="B34">
-            <v>4.0999999999999996</v>
-          </cell>
-          <cell r="C34">
-            <v>1.5</v>
-          </cell>
-          <cell r="D34">
-            <v>0.1</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="A35">
-            <v>5.5</v>
-          </cell>
-          <cell r="B35">
-            <v>4.2</v>
-          </cell>
-          <cell r="C35">
-            <v>1.4</v>
-          </cell>
-          <cell r="D35">
-            <v>0.2</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="A36">
-            <v>4.9000000000000004</v>
-          </cell>
-          <cell r="B36">
-            <v>3.1</v>
-          </cell>
-          <cell r="C36">
-            <v>1.5</v>
-          </cell>
-          <cell r="D36">
-            <v>0.1</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="A37">
-            <v>5</v>
-          </cell>
-          <cell r="B37">
-            <v>3.2</v>
-          </cell>
-          <cell r="C37">
-            <v>1.2</v>
-          </cell>
-          <cell r="D37">
-            <v>0.2</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="A38">
-            <v>5.5</v>
-          </cell>
-          <cell r="B38">
-            <v>3.5</v>
-          </cell>
-          <cell r="C38">
-            <v>1.3</v>
-          </cell>
-          <cell r="D38">
-            <v>0.2</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="A39">
-            <v>4.9000000000000004</v>
-          </cell>
-          <cell r="B39">
-            <v>3.1</v>
-          </cell>
-          <cell r="C39">
-            <v>1.5</v>
-          </cell>
-          <cell r="D39">
-            <v>0.1</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="A40">
-            <v>4.4000000000000004</v>
-          </cell>
-          <cell r="B40">
-            <v>3</v>
-          </cell>
-          <cell r="C40">
-            <v>1.3</v>
-          </cell>
-          <cell r="D40">
-            <v>0.2</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="A41">
-            <v>5.0999999999999996</v>
-          </cell>
-          <cell r="B41">
-            <v>3.4</v>
-          </cell>
-          <cell r="C41">
-            <v>1.5</v>
-          </cell>
-          <cell r="D41">
-            <v>0.2</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="A42">
-            <v>5</v>
-          </cell>
-          <cell r="B42">
-            <v>3.5</v>
-          </cell>
-          <cell r="C42">
-            <v>1.3</v>
-          </cell>
-          <cell r="D42">
-            <v>0.3</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="A43">
-            <v>4.5</v>
-          </cell>
-          <cell r="B43">
-            <v>2.2999999999999998</v>
-          </cell>
-          <cell r="C43">
-            <v>1.3</v>
-          </cell>
-          <cell r="D43">
-            <v>0.3</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="A44">
-            <v>4.4000000000000004</v>
-          </cell>
-          <cell r="B44">
-            <v>3.2</v>
-          </cell>
-          <cell r="C44">
-            <v>1.3</v>
-          </cell>
-          <cell r="D44">
-            <v>0.2</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="A45">
-            <v>5</v>
-          </cell>
-          <cell r="B45">
-            <v>3.5</v>
-          </cell>
-          <cell r="C45">
-            <v>1.6</v>
-          </cell>
-          <cell r="D45">
-            <v>0.6</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="A46">
-            <v>5.0999999999999996</v>
-          </cell>
-          <cell r="B46">
-            <v>3.8</v>
-          </cell>
-          <cell r="C46">
-            <v>1.9</v>
-          </cell>
-          <cell r="D46">
-            <v>0.4</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="A47">
-            <v>4.8</v>
-          </cell>
-          <cell r="B47">
-            <v>3</v>
-          </cell>
-          <cell r="C47">
-            <v>1.4</v>
-          </cell>
-          <cell r="D47">
-            <v>0.3</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="A48">
-            <v>5.0999999999999996</v>
-          </cell>
-          <cell r="B48">
-            <v>3.8</v>
-          </cell>
-          <cell r="C48">
-            <v>1.6</v>
-          </cell>
-          <cell r="D48">
-            <v>0.2</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="A49">
-            <v>4.5999999999999996</v>
-          </cell>
-          <cell r="B49">
-            <v>3.2</v>
-          </cell>
-          <cell r="C49">
-            <v>1.4</v>
-          </cell>
-          <cell r="D49">
-            <v>0.2</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="A50">
-            <v>5.3</v>
-          </cell>
-          <cell r="B50">
-            <v>3.7</v>
-          </cell>
-          <cell r="C50">
-            <v>1.5</v>
-          </cell>
-          <cell r="D50">
-            <v>0.2</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="A51">
-            <v>5</v>
-          </cell>
-          <cell r="B51">
-            <v>3.3</v>
-          </cell>
-          <cell r="C51">
-            <v>1.4</v>
-          </cell>
-          <cell r="D51">
-            <v>0.2</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="A52">
-            <v>7</v>
-          </cell>
-          <cell r="B52">
-            <v>3.2</v>
-          </cell>
-          <cell r="C52">
-            <v>4.7</v>
-          </cell>
-          <cell r="D52">
-            <v>1.4</v>
-          </cell>
-          <cell r="E52" t="str">
-            <v>iris_versicolor</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="A53">
-            <v>6.4</v>
-          </cell>
-          <cell r="B53">
-            <v>3.2</v>
-          </cell>
-          <cell r="C53">
-            <v>4.5</v>
-          </cell>
-          <cell r="D53">
-            <v>1.5</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="A54">
-            <v>6.9</v>
-          </cell>
-          <cell r="B54">
-            <v>3.1</v>
-          </cell>
-          <cell r="C54">
-            <v>4.9000000000000004</v>
-          </cell>
-          <cell r="D54">
-            <v>1.5</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="A55">
-            <v>5.5</v>
-          </cell>
-          <cell r="B55">
-            <v>2.2999999999999998</v>
-          </cell>
-          <cell r="C55">
-            <v>4</v>
-          </cell>
-          <cell r="D55">
-            <v>1.3</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="A56">
-            <v>6.5</v>
-          </cell>
-          <cell r="B56">
-            <v>2.8</v>
-          </cell>
-          <cell r="C56">
-            <v>4.5999999999999996</v>
-          </cell>
-          <cell r="D56">
-            <v>1.5</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="A57">
-            <v>5.7</v>
-          </cell>
-          <cell r="B57">
-            <v>2.8</v>
-          </cell>
-          <cell r="C57">
-            <v>4.5</v>
-          </cell>
-          <cell r="D57">
-            <v>1.3</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="A58">
-            <v>6.3</v>
-          </cell>
-          <cell r="B58">
-            <v>3.3</v>
-          </cell>
-          <cell r="C58">
-            <v>4.7</v>
-          </cell>
-          <cell r="D58">
-            <v>1.6</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="A59">
-            <v>4.9000000000000004</v>
-          </cell>
-          <cell r="B59">
-            <v>2.4</v>
-          </cell>
-          <cell r="C59">
-            <v>3.3</v>
-          </cell>
-          <cell r="D59">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="A60">
-            <v>6.6</v>
-          </cell>
-          <cell r="B60">
-            <v>2.9</v>
-          </cell>
-          <cell r="C60">
-            <v>4.5999999999999996</v>
-          </cell>
-          <cell r="D60">
-            <v>1.3</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="A61">
-            <v>5.2</v>
-          </cell>
-          <cell r="B61">
-            <v>2.7</v>
-          </cell>
-          <cell r="C61">
-            <v>3.9</v>
-          </cell>
-          <cell r="D61">
-            <v>1.4</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="A62">
-            <v>5</v>
-          </cell>
-          <cell r="B62">
-            <v>2</v>
-          </cell>
-          <cell r="C62">
-            <v>3.5</v>
-          </cell>
-          <cell r="D62">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="A63">
-            <v>5.9</v>
-          </cell>
-          <cell r="B63">
-            <v>3</v>
-          </cell>
-          <cell r="C63">
-            <v>4.2</v>
-          </cell>
-          <cell r="D63">
-            <v>1.5</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="A64">
-            <v>6</v>
-          </cell>
-          <cell r="B64">
-            <v>2.2000000000000002</v>
-          </cell>
-          <cell r="C64">
-            <v>4</v>
-          </cell>
-          <cell r="D64">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="65">
-          <cell r="A65">
-            <v>6.1</v>
-          </cell>
-          <cell r="B65">
-            <v>2.9</v>
-          </cell>
-          <cell r="C65">
-            <v>4.7</v>
-          </cell>
-          <cell r="D65">
-            <v>1.4</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="A66">
-            <v>5.6</v>
-          </cell>
-          <cell r="B66">
-            <v>2.9</v>
-          </cell>
-          <cell r="C66">
-            <v>3.6</v>
-          </cell>
-          <cell r="D66">
-            <v>1.3</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="A67">
-            <v>6.7</v>
-          </cell>
-          <cell r="B67">
-            <v>3.1</v>
-          </cell>
-          <cell r="C67">
-            <v>4.4000000000000004</v>
-          </cell>
-          <cell r="D67">
-            <v>1.4</v>
-          </cell>
-        </row>
-        <row r="68">
-          <cell r="A68">
-            <v>5.6</v>
-          </cell>
-          <cell r="B68">
-            <v>3</v>
-          </cell>
-          <cell r="C68">
-            <v>4.5</v>
-          </cell>
-          <cell r="D68">
-            <v>1.5</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="A69">
-            <v>5.8</v>
-          </cell>
-          <cell r="B69">
-            <v>2.7</v>
-          </cell>
-          <cell r="C69">
-            <v>4.0999999999999996</v>
-          </cell>
-          <cell r="D69">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="A70">
-            <v>6.2</v>
-          </cell>
-          <cell r="B70">
-            <v>2.2000000000000002</v>
-          </cell>
-          <cell r="C70">
-            <v>4.5</v>
-          </cell>
-          <cell r="D70">
-            <v>1.5</v>
-          </cell>
-        </row>
-        <row r="71">
-          <cell r="A71">
-            <v>5.6</v>
-          </cell>
-          <cell r="B71">
-            <v>2.5</v>
-          </cell>
-          <cell r="C71">
-            <v>3.9</v>
-          </cell>
-          <cell r="D71">
-            <v>1.1000000000000001</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="A72">
-            <v>5.9</v>
-          </cell>
-          <cell r="B72">
-            <v>3.2</v>
-          </cell>
-          <cell r="C72">
-            <v>4.8</v>
-          </cell>
-          <cell r="D72">
-            <v>1.8</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="A73">
-            <v>6.1</v>
-          </cell>
-          <cell r="B73">
-            <v>2.8</v>
-          </cell>
-          <cell r="C73">
-            <v>4</v>
-          </cell>
-          <cell r="D73">
-            <v>1.3</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="A74">
-            <v>6.3</v>
-          </cell>
-          <cell r="B74">
-            <v>2.5</v>
-          </cell>
-          <cell r="C74">
-            <v>4.9000000000000004</v>
-          </cell>
-          <cell r="D74">
-            <v>1.5</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="A75">
-            <v>6.1</v>
-          </cell>
-          <cell r="B75">
-            <v>2.8</v>
-          </cell>
-          <cell r="C75">
-            <v>4.7</v>
-          </cell>
-          <cell r="D75">
-            <v>1.2</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="A76">
-            <v>6.4</v>
-          </cell>
-          <cell r="B76">
-            <v>2.9</v>
-          </cell>
-          <cell r="C76">
-            <v>4.3</v>
-          </cell>
-          <cell r="D76">
-            <v>1.3</v>
-          </cell>
-        </row>
-        <row r="77">
-          <cell r="A77">
-            <v>6.6</v>
-          </cell>
-          <cell r="B77">
-            <v>3</v>
-          </cell>
-          <cell r="C77">
-            <v>4.4000000000000004</v>
-          </cell>
-          <cell r="D77">
-            <v>1.4</v>
-          </cell>
-        </row>
-        <row r="78">
-          <cell r="A78">
-            <v>6.8</v>
-          </cell>
-          <cell r="B78">
-            <v>2.8</v>
-          </cell>
-          <cell r="C78">
-            <v>4.8</v>
-          </cell>
-          <cell r="D78">
-            <v>1.4</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="A79">
-            <v>6.7</v>
-          </cell>
-          <cell r="B79">
-            <v>3</v>
-          </cell>
-          <cell r="C79">
-            <v>5</v>
-          </cell>
-          <cell r="D79">
-            <v>1.7</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="A80">
-            <v>6</v>
-          </cell>
-          <cell r="B80">
-            <v>2.9</v>
-          </cell>
-          <cell r="C80">
-            <v>4.5</v>
-          </cell>
-          <cell r="D80">
-            <v>1.5</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="A81">
-            <v>5.7</v>
-          </cell>
-          <cell r="B81">
-            <v>2.6</v>
-          </cell>
-          <cell r="C81">
-            <v>3.5</v>
-          </cell>
-          <cell r="D81">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="82">
-          <cell r="A82">
-            <v>5.5</v>
-          </cell>
-          <cell r="B82">
-            <v>2.4</v>
-          </cell>
-          <cell r="C82">
-            <v>3.8</v>
-          </cell>
-          <cell r="D82">
-            <v>1.1000000000000001</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="A83">
-            <v>5.5</v>
-          </cell>
-          <cell r="B83">
-            <v>2.4</v>
-          </cell>
-          <cell r="C83">
-            <v>3.7</v>
-          </cell>
-          <cell r="D83">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="84">
-          <cell r="A84">
-            <v>5.8</v>
-          </cell>
-          <cell r="B84">
-            <v>2.7</v>
-          </cell>
-          <cell r="C84">
-            <v>3.9</v>
-          </cell>
-          <cell r="D84">
-            <v>1.2</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="A85">
-            <v>6</v>
-          </cell>
-          <cell r="B85">
-            <v>2.7</v>
-          </cell>
-          <cell r="C85">
-            <v>5.0999999999999996</v>
-          </cell>
-          <cell r="D85">
-            <v>1.6</v>
-          </cell>
-        </row>
-        <row r="86">
-          <cell r="A86">
-            <v>5.4</v>
-          </cell>
-          <cell r="B86">
-            <v>3</v>
-          </cell>
-          <cell r="C86">
-            <v>4.5</v>
-          </cell>
-          <cell r="D86">
-            <v>1.5</v>
-          </cell>
-        </row>
-        <row r="87">
-          <cell r="A87">
-            <v>6</v>
-          </cell>
-          <cell r="B87">
-            <v>3.4</v>
-          </cell>
-          <cell r="C87">
-            <v>4.5</v>
-          </cell>
-          <cell r="D87">
-            <v>1.6</v>
-          </cell>
-        </row>
-        <row r="88">
-          <cell r="A88">
-            <v>6.7</v>
-          </cell>
-          <cell r="B88">
-            <v>3.1</v>
-          </cell>
-          <cell r="C88">
-            <v>4.7</v>
-          </cell>
-          <cell r="D88">
-            <v>1.5</v>
-          </cell>
-        </row>
-        <row r="89">
-          <cell r="A89">
-            <v>6.3</v>
-          </cell>
-          <cell r="B89">
-            <v>2.2999999999999998</v>
-          </cell>
-          <cell r="C89">
-            <v>4.4000000000000004</v>
-          </cell>
-          <cell r="D89">
-            <v>1.3</v>
-          </cell>
-        </row>
-        <row r="90">
-          <cell r="A90">
-            <v>5.6</v>
-          </cell>
-          <cell r="B90">
-            <v>3</v>
-          </cell>
-          <cell r="C90">
-            <v>4.0999999999999996</v>
-          </cell>
-          <cell r="D90">
-            <v>1.3</v>
-          </cell>
-        </row>
-        <row r="91">
-          <cell r="A91">
-            <v>5.5</v>
-          </cell>
-          <cell r="B91">
-            <v>2.5</v>
-          </cell>
-          <cell r="C91">
-            <v>4</v>
-          </cell>
-          <cell r="D91">
-            <v>1.3</v>
-          </cell>
-        </row>
-        <row r="92">
-          <cell r="A92">
-            <v>5.5</v>
-          </cell>
-          <cell r="B92">
-            <v>2.6</v>
-          </cell>
-          <cell r="C92">
-            <v>4.4000000000000004</v>
-          </cell>
-          <cell r="D92">
-            <v>1.2</v>
-          </cell>
-        </row>
-        <row r="93">
-          <cell r="A93">
-            <v>6.1</v>
-          </cell>
-          <cell r="B93">
-            <v>3</v>
-          </cell>
-          <cell r="C93">
-            <v>4.5999999999999996</v>
-          </cell>
-          <cell r="D93">
-            <v>1.4</v>
-          </cell>
-        </row>
-        <row r="94">
-          <cell r="A94">
-            <v>5.8</v>
-          </cell>
-          <cell r="B94">
-            <v>2.6</v>
-          </cell>
-          <cell r="C94">
-            <v>4</v>
-          </cell>
-          <cell r="D94">
-            <v>1.2</v>
-          </cell>
-        </row>
-        <row r="95">
-          <cell r="A95">
-            <v>5</v>
-          </cell>
-          <cell r="B95">
-            <v>2.2999999999999998</v>
-          </cell>
-          <cell r="C95">
-            <v>3.3</v>
-          </cell>
-          <cell r="D95">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="96">
-          <cell r="A96">
-            <v>5.6</v>
-          </cell>
-          <cell r="B96">
-            <v>2.7</v>
-          </cell>
-          <cell r="C96">
-            <v>4.2</v>
-          </cell>
-          <cell r="D96">
-            <v>1.3</v>
-          </cell>
-        </row>
-        <row r="97">
-          <cell r="A97">
-            <v>5.7</v>
-          </cell>
-          <cell r="B97">
-            <v>3</v>
-          </cell>
-          <cell r="C97">
-            <v>4.2</v>
-          </cell>
-          <cell r="D97">
-            <v>1.2</v>
-          </cell>
-        </row>
-        <row r="98">
-          <cell r="A98">
-            <v>5.7</v>
-          </cell>
-          <cell r="B98">
-            <v>2.9</v>
-          </cell>
-          <cell r="C98">
-            <v>4.2</v>
-          </cell>
-          <cell r="D98">
-            <v>1.3</v>
-          </cell>
-        </row>
-        <row r="99">
-          <cell r="A99">
-            <v>6.2</v>
-          </cell>
-          <cell r="B99">
-            <v>2.9</v>
-          </cell>
-          <cell r="C99">
-            <v>4.3</v>
-          </cell>
-          <cell r="D99">
-            <v>1.3</v>
-          </cell>
-        </row>
-        <row r="100">
-          <cell r="A100">
-            <v>5.0999999999999996</v>
-          </cell>
-          <cell r="B100">
-            <v>2.5</v>
-          </cell>
-          <cell r="C100">
-            <v>3</v>
-          </cell>
-          <cell r="D100">
-            <v>1.1000000000000001</v>
-          </cell>
-        </row>
-        <row r="101">
-          <cell r="A101">
-            <v>5.7</v>
-          </cell>
-          <cell r="B101">
-            <v>2.8</v>
-          </cell>
-          <cell r="C101">
-            <v>4.0999999999999996</v>
-          </cell>
-          <cell r="D101">
-            <v>1.3</v>
-          </cell>
-        </row>
-        <row r="102">
-          <cell r="A102">
-            <v>6.3</v>
-          </cell>
-          <cell r="B102">
-            <v>3.3</v>
-          </cell>
-          <cell r="C102">
-            <v>6</v>
-          </cell>
-          <cell r="D102">
-            <v>2.5</v>
-          </cell>
-          <cell r="E102" t="str">
-            <v>iris_virginica</v>
-          </cell>
-        </row>
-        <row r="103">
-          <cell r="A103">
-            <v>5.8</v>
-          </cell>
-          <cell r="B103">
-            <v>2.7</v>
-          </cell>
-          <cell r="C103">
-            <v>5.0999999999999996</v>
-          </cell>
-          <cell r="D103">
-            <v>1.9</v>
-          </cell>
-        </row>
-        <row r="104">
-          <cell r="A104">
-            <v>7.1</v>
-          </cell>
-          <cell r="B104">
-            <v>3</v>
-          </cell>
-          <cell r="C104">
-            <v>5.9</v>
-          </cell>
-          <cell r="D104">
-            <v>2.1</v>
-          </cell>
-        </row>
-        <row r="105">
-          <cell r="A105">
-            <v>6.3</v>
-          </cell>
-          <cell r="B105">
-            <v>2.9</v>
-          </cell>
-          <cell r="C105">
-            <v>5.6</v>
-          </cell>
-          <cell r="D105">
-            <v>1.8</v>
-          </cell>
-        </row>
-        <row r="106">
-          <cell r="A106">
-            <v>6.5</v>
-          </cell>
-          <cell r="B106">
-            <v>3</v>
-          </cell>
-          <cell r="C106">
-            <v>5.8</v>
-          </cell>
-          <cell r="D106">
-            <v>2.2000000000000002</v>
-          </cell>
-        </row>
-        <row r="107">
-          <cell r="A107">
-            <v>7.6</v>
-          </cell>
-          <cell r="B107">
-            <v>3</v>
-          </cell>
-          <cell r="C107">
-            <v>6.6</v>
-          </cell>
-          <cell r="D107">
-            <v>2.1</v>
-          </cell>
-        </row>
-        <row r="108">
-          <cell r="A108">
-            <v>4.9000000000000004</v>
-          </cell>
-          <cell r="B108">
-            <v>2.5</v>
-          </cell>
-          <cell r="C108">
-            <v>4.5</v>
-          </cell>
-          <cell r="D108">
-            <v>1.7</v>
-          </cell>
-        </row>
-        <row r="109">
-          <cell r="A109">
-            <v>7.3</v>
-          </cell>
-          <cell r="B109">
-            <v>2.9</v>
-          </cell>
-          <cell r="C109">
-            <v>6.3</v>
-          </cell>
-          <cell r="D109">
-            <v>1.8</v>
-          </cell>
-        </row>
-        <row r="110">
-          <cell r="A110">
-            <v>6.7</v>
-          </cell>
-          <cell r="B110">
-            <v>2.5</v>
-          </cell>
-          <cell r="C110">
-            <v>5.8</v>
-          </cell>
-          <cell r="D110">
-            <v>1.8</v>
-          </cell>
-        </row>
-        <row r="111">
-          <cell r="A111">
-            <v>7.2</v>
-          </cell>
-          <cell r="B111">
-            <v>3.6</v>
-          </cell>
-          <cell r="C111">
-            <v>6.1</v>
-          </cell>
-          <cell r="D111">
-            <v>2.5</v>
-          </cell>
-        </row>
-        <row r="112">
-          <cell r="A112">
-            <v>6.5</v>
-          </cell>
-          <cell r="B112">
-            <v>3.2</v>
-          </cell>
-          <cell r="C112">
-            <v>5.0999999999999996</v>
-          </cell>
-          <cell r="D112">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="113">
-          <cell r="A113">
-            <v>6.4</v>
-          </cell>
-          <cell r="B113">
-            <v>2.7</v>
-          </cell>
-          <cell r="C113">
-            <v>5.3</v>
-          </cell>
-          <cell r="D113">
-            <v>1.9</v>
-          </cell>
-        </row>
-        <row r="114">
-          <cell r="A114">
-            <v>6.8</v>
-          </cell>
-          <cell r="B114">
-            <v>3</v>
-          </cell>
-          <cell r="C114">
-            <v>5.5</v>
-          </cell>
-          <cell r="D114">
-            <v>2.1</v>
-          </cell>
-        </row>
-        <row r="115">
-          <cell r="A115">
-            <v>5.7</v>
-          </cell>
-          <cell r="B115">
-            <v>2.5</v>
-          </cell>
-          <cell r="C115">
-            <v>5</v>
-          </cell>
-          <cell r="D115">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="116">
-          <cell r="A116">
-            <v>5.8</v>
-          </cell>
-          <cell r="B116">
-            <v>2.8</v>
-          </cell>
-          <cell r="C116">
-            <v>5.0999999999999996</v>
-          </cell>
-          <cell r="D116">
-            <v>2.4</v>
-          </cell>
-        </row>
-        <row r="117">
-          <cell r="A117">
-            <v>6.4</v>
-          </cell>
-          <cell r="B117">
-            <v>3.2</v>
-          </cell>
-          <cell r="C117">
-            <v>5.3</v>
-          </cell>
-          <cell r="D117">
-            <v>2.2999999999999998</v>
-          </cell>
-        </row>
-        <row r="118">
-          <cell r="A118">
-            <v>6.5</v>
-          </cell>
-          <cell r="B118">
-            <v>3</v>
-          </cell>
-          <cell r="C118">
-            <v>5.5</v>
-          </cell>
-          <cell r="D118">
-            <v>1.8</v>
-          </cell>
-        </row>
-        <row r="119">
-          <cell r="A119">
-            <v>7.7</v>
-          </cell>
-          <cell r="B119">
-            <v>3.8</v>
-          </cell>
-          <cell r="C119">
-            <v>6.7</v>
-          </cell>
-          <cell r="D119">
-            <v>2.2000000000000002</v>
-          </cell>
-        </row>
-        <row r="120">
-          <cell r="A120">
-            <v>7.7</v>
-          </cell>
-          <cell r="B120">
-            <v>2.6</v>
-          </cell>
-          <cell r="C120">
-            <v>6.9</v>
-          </cell>
-          <cell r="D120">
-            <v>2.2999999999999998</v>
-          </cell>
-        </row>
-        <row r="121">
-          <cell r="A121">
-            <v>6</v>
-          </cell>
-          <cell r="B121">
-            <v>2.2000000000000002</v>
-          </cell>
-          <cell r="C121">
-            <v>5</v>
-          </cell>
-          <cell r="D121">
-            <v>1.5</v>
-          </cell>
-        </row>
-        <row r="122">
-          <cell r="A122">
-            <v>6.9</v>
-          </cell>
-          <cell r="B122">
-            <v>3.2</v>
-          </cell>
-          <cell r="C122">
-            <v>5.7</v>
-          </cell>
-          <cell r="D122">
-            <v>2.2999999999999998</v>
-          </cell>
-        </row>
-        <row r="123">
-          <cell r="A123">
-            <v>5.6</v>
-          </cell>
-          <cell r="B123">
-            <v>2.8</v>
-          </cell>
-          <cell r="C123">
-            <v>4.9000000000000004</v>
-          </cell>
-          <cell r="D123">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="124">
-          <cell r="A124">
-            <v>7.7</v>
-          </cell>
-          <cell r="B124">
-            <v>2.8</v>
-          </cell>
-          <cell r="C124">
-            <v>6.7</v>
-          </cell>
-          <cell r="D124">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="125">
-          <cell r="A125">
-            <v>6.3</v>
-          </cell>
-          <cell r="B125">
-            <v>2.7</v>
-          </cell>
-          <cell r="C125">
-            <v>4.9000000000000004</v>
-          </cell>
-          <cell r="D125">
-            <v>1.8</v>
-          </cell>
-        </row>
-        <row r="126">
-          <cell r="A126">
-            <v>6.7</v>
-          </cell>
-          <cell r="B126">
-            <v>3.3</v>
-          </cell>
-          <cell r="C126">
-            <v>5.7</v>
-          </cell>
-          <cell r="D126">
-            <v>2.1</v>
-          </cell>
-        </row>
-        <row r="127">
-          <cell r="A127">
-            <v>7.2</v>
-          </cell>
-          <cell r="B127">
-            <v>3.2</v>
-          </cell>
-          <cell r="C127">
-            <v>6</v>
-          </cell>
-          <cell r="D127">
-            <v>1.8</v>
-          </cell>
-        </row>
-        <row r="128">
-          <cell r="A128">
-            <v>6.2</v>
-          </cell>
-          <cell r="B128">
-            <v>2.8</v>
-          </cell>
-          <cell r="C128">
-            <v>4.8</v>
-          </cell>
-          <cell r="D128">
-            <v>1.8</v>
-          </cell>
-        </row>
-        <row r="129">
-          <cell r="A129">
-            <v>6.1</v>
-          </cell>
-          <cell r="B129">
-            <v>3</v>
-          </cell>
-          <cell r="C129">
-            <v>4.9000000000000004</v>
-          </cell>
-          <cell r="D129">
-            <v>1.8</v>
-          </cell>
-        </row>
-        <row r="130">
-          <cell r="A130">
-            <v>6.4</v>
-          </cell>
-          <cell r="B130">
-            <v>2.8</v>
-          </cell>
-          <cell r="C130">
-            <v>5.6</v>
-          </cell>
-          <cell r="D130">
-            <v>2.1</v>
-          </cell>
-        </row>
-        <row r="131">
-          <cell r="A131">
-            <v>7.2</v>
-          </cell>
-          <cell r="B131">
-            <v>3</v>
-          </cell>
-          <cell r="C131">
-            <v>5.8</v>
-          </cell>
-          <cell r="D131">
-            <v>1.6</v>
-          </cell>
-        </row>
-        <row r="132">
-          <cell r="A132">
-            <v>7.4</v>
-          </cell>
-          <cell r="B132">
-            <v>2.8</v>
-          </cell>
-          <cell r="C132">
-            <v>6.1</v>
-          </cell>
-          <cell r="D132">
-            <v>1.9</v>
-          </cell>
-        </row>
-        <row r="133">
-          <cell r="A133">
-            <v>7.9</v>
-          </cell>
-          <cell r="B133">
-            <v>3.8</v>
-          </cell>
-          <cell r="C133">
-            <v>6.4</v>
-          </cell>
-          <cell r="D133">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="134">
-          <cell r="A134">
-            <v>6.4</v>
-          </cell>
-          <cell r="B134">
-            <v>2.8</v>
-          </cell>
-          <cell r="C134">
-            <v>5.6</v>
-          </cell>
-          <cell r="D134">
-            <v>2.2000000000000002</v>
-          </cell>
-        </row>
-        <row r="135">
-          <cell r="A135">
-            <v>6.3</v>
-          </cell>
-          <cell r="B135">
-            <v>2.8</v>
-          </cell>
-          <cell r="C135">
-            <v>5.0999999999999996</v>
-          </cell>
-          <cell r="D135">
-            <v>1.5</v>
-          </cell>
-        </row>
-        <row r="136">
-          <cell r="A136">
-            <v>6.1</v>
-          </cell>
-          <cell r="B136">
-            <v>2.6</v>
-          </cell>
-          <cell r="C136">
-            <v>5.6</v>
-          </cell>
-          <cell r="D136">
-            <v>1.4</v>
-          </cell>
-        </row>
-        <row r="137">
-          <cell r="A137">
-            <v>7.7</v>
-          </cell>
-          <cell r="B137">
-            <v>3</v>
-          </cell>
-          <cell r="C137">
-            <v>6.1</v>
-          </cell>
-          <cell r="D137">
-            <v>2.2999999999999998</v>
-          </cell>
-        </row>
-        <row r="138">
-          <cell r="A138">
-            <v>6.3</v>
-          </cell>
-          <cell r="B138">
-            <v>3.4</v>
-          </cell>
-          <cell r="C138">
-            <v>5.6</v>
-          </cell>
-          <cell r="D138">
-            <v>2.4</v>
-          </cell>
-        </row>
-        <row r="139">
-          <cell r="A139">
-            <v>6.4</v>
-          </cell>
-          <cell r="B139">
-            <v>3.1</v>
-          </cell>
-          <cell r="C139">
-            <v>5.5</v>
-          </cell>
-          <cell r="D139">
-            <v>1.8</v>
-          </cell>
-        </row>
-        <row r="140">
-          <cell r="A140">
-            <v>6</v>
-          </cell>
-          <cell r="B140">
-            <v>3</v>
-          </cell>
-          <cell r="C140">
-            <v>4.8</v>
-          </cell>
-          <cell r="D140">
-            <v>1.8</v>
-          </cell>
-        </row>
-        <row r="141">
-          <cell r="A141">
-            <v>6.9</v>
-          </cell>
-          <cell r="B141">
-            <v>3.1</v>
-          </cell>
-          <cell r="C141">
-            <v>5.4</v>
-          </cell>
-          <cell r="D141">
-            <v>2.1</v>
-          </cell>
-        </row>
-        <row r="142">
-          <cell r="A142">
-            <v>6.7</v>
-          </cell>
-          <cell r="B142">
-            <v>3.1</v>
-          </cell>
-          <cell r="C142">
-            <v>5.6</v>
-          </cell>
-          <cell r="D142">
-            <v>2.4</v>
-          </cell>
-        </row>
-        <row r="143">
-          <cell r="A143">
-            <v>6.9</v>
-          </cell>
-          <cell r="B143">
-            <v>3.1</v>
-          </cell>
-          <cell r="C143">
-            <v>5.0999999999999996</v>
-          </cell>
-          <cell r="D143">
-            <v>2.2999999999999998</v>
-          </cell>
-        </row>
-        <row r="144">
-          <cell r="A144">
-            <v>5.8</v>
-          </cell>
-          <cell r="B144">
-            <v>2.7</v>
-          </cell>
-          <cell r="C144">
-            <v>5.0999999999999996</v>
-          </cell>
-          <cell r="D144">
-            <v>1.9</v>
-          </cell>
-        </row>
-        <row r="145">
-          <cell r="A145">
-            <v>6.8</v>
-          </cell>
-          <cell r="B145">
-            <v>3.2</v>
-          </cell>
-          <cell r="C145">
-            <v>5.9</v>
-          </cell>
-          <cell r="D145">
-            <v>2.2999999999999998</v>
-          </cell>
-        </row>
-        <row r="146">
-          <cell r="A146">
-            <v>6.7</v>
-          </cell>
-          <cell r="B146">
-            <v>3.3</v>
-          </cell>
-          <cell r="C146">
-            <v>5.7</v>
-          </cell>
-          <cell r="D146">
-            <v>2.5</v>
-          </cell>
-        </row>
-        <row r="147">
-          <cell r="A147">
-            <v>6.7</v>
-          </cell>
-          <cell r="B147">
-            <v>3</v>
-          </cell>
-          <cell r="C147">
-            <v>5.2</v>
-          </cell>
-          <cell r="D147">
-            <v>2.2999999999999998</v>
-          </cell>
-        </row>
-        <row r="148">
-          <cell r="A148">
-            <v>6.3</v>
-          </cell>
-          <cell r="B148">
-            <v>2.5</v>
-          </cell>
-          <cell r="C148">
-            <v>5</v>
-          </cell>
-          <cell r="D148">
-            <v>1.9</v>
-          </cell>
-        </row>
-        <row r="149">
-          <cell r="A149">
-            <v>6.5</v>
-          </cell>
-          <cell r="B149">
-            <v>3</v>
-          </cell>
-          <cell r="C149">
-            <v>5.2</v>
-          </cell>
-          <cell r="D149">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="150">
-          <cell r="A150">
-            <v>6.2</v>
-          </cell>
-          <cell r="B150">
-            <v>3.4</v>
-          </cell>
-          <cell r="C150">
-            <v>5.4</v>
-          </cell>
-          <cell r="D150">
-            <v>2.2999999999999998</v>
-          </cell>
-        </row>
-        <row r="151">
-          <cell r="A151">
-            <v>5.9</v>
-          </cell>
-          <cell r="B151">
-            <v>3</v>
-          </cell>
-          <cell r="C151">
-            <v>5.0999999999999996</v>
-          </cell>
-          <cell r="D151">
-            <v>1.8</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18320,11 +18129,634 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BF074EF-15E7-4415-931A-35AE88D56480}">
+  <dimension ref="B2:AH37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="35"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="B2" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="C5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="35">
+        <v>0.15</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="35">
+        <v>0.4</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="V5" s="35">
+        <v>0.15</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA5" s="35">
+        <v>0.4</v>
+      </c>
+      <c r="AC5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG5" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="C6" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="G6" s="6">
+        <f>C6*E5+C12*E10+C18*D14</f>
+        <v>0.3775</v>
+      </c>
+      <c r="H6" s="6">
+        <f>1/(1+EXP(-G6))</f>
+        <v>0.59326999210718723</v>
+      </c>
+      <c r="L6" s="6">
+        <f>H6*J5+H12*J10+H18*I14</f>
+        <v>1.10590596705977</v>
+      </c>
+      <c r="M6" s="6">
+        <f>1/(1+EXP(-L6))</f>
+        <v>0.75136506955231575</v>
+      </c>
+      <c r="O6" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="P6" s="6">
+        <f>(O6-M6)^2</f>
+        <v>0.54962216635230998</v>
+      </c>
+      <c r="T6" s="6">
+        <v>0.08</v>
+      </c>
+      <c r="X6" s="6">
+        <f>T6*V5+T12*V10+T18*U14</f>
+        <v>0.39199999999999996</v>
+      </c>
+      <c r="Y6" s="6">
+        <f>1/(1+EXP(-X6))</f>
+        <v>0.59676406572544638</v>
+      </c>
+      <c r="AC6" s="6">
+        <f>Y6*AA5+Y12*AA10+Y18*Z14</f>
+        <v>1.1097344058900624</v>
+      </c>
+      <c r="AD6" s="6">
+        <f>1/(1+EXP(-AC6))</f>
+        <v>0.75207959317200401</v>
+      </c>
+      <c r="AF6" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="AG6" s="6">
+        <f>(AF6-AD6)^2</f>
+        <v>0.53594053073888692</v>
+      </c>
+    </row>
+    <row r="7" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="D7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="35">
+        <v>0.25</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="U7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="V7" s="35">
+        <v>0.25</v>
+      </c>
+      <c r="Z7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA7" s="35">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="Q8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AH8" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="Q9" s="6">
+        <f>(P6+P12)/2</f>
+        <v>0.29837110876000272</v>
+      </c>
+      <c r="AH9" s="6">
+        <f>(AG6+AG12)/2</f>
+        <v>0.28350133433011626</v>
+      </c>
+    </row>
+    <row r="10" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="D10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="35">
+        <v>0.2</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="35">
+        <v>0.45</v>
+      </c>
+      <c r="U10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="V10" s="35">
+        <v>0.2</v>
+      </c>
+      <c r="Z10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA10" s="35">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="11" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="C11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="T11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="X11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG11" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="C12" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="35">
+        <v>0.3</v>
+      </c>
+      <c r="G12" s="6">
+        <f>C6*E7+C12*E12+C18*E15</f>
+        <v>0.39249999999999996</v>
+      </c>
+      <c r="H12" s="6">
+        <f>1/(1+EXP(-G12))</f>
+        <v>0.59688437825976703</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" s="35">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L12" s="6">
+        <f>H6*J7+H12*J12+H18*J15</f>
+        <v>1.2249214040964653</v>
+      </c>
+      <c r="M12" s="6">
+        <f>1/(1+EXP(-L12))</f>
+        <v>0.77292846532146253</v>
+      </c>
+      <c r="O12" s="6">
+        <v>0.99</v>
+      </c>
+      <c r="P12" s="6">
+        <f>(O12-M12)^2</f>
+        <v>4.7120051167695493E-2</v>
+      </c>
+      <c r="T12" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="U12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="V12" s="35">
+        <v>0.3</v>
+      </c>
+      <c r="X12" s="6">
+        <f>T6*V7+T12*V12+T18*V15</f>
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="Y12" s="6">
+        <f>1/(1+EXP(-X12))</f>
+        <v>0.60228617688863062</v>
+      </c>
+      <c r="Z12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA12" s="35">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="AC12" s="6">
+        <f>Y6*AA7+Y12*AA12+Y18*AA15</f>
+        <v>1.2296394301514701</v>
+      </c>
+      <c r="AD12" s="6">
+        <f>1/(1+EXP(-AC12))</f>
+        <v>0.77375545988216943</v>
+      </c>
+      <c r="AF12" s="6">
+        <v>0.95</v>
+      </c>
+      <c r="AG12" s="6">
+        <f>(AF12-AD12)^2</f>
+        <v>3.1062137921345573E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="D14" s="35">
+        <v>0.35</v>
+      </c>
+      <c r="I14" s="35">
+        <v>0.6</v>
+      </c>
+      <c r="U14" s="35">
+        <v>0.35</v>
+      </c>
+      <c r="Z14" s="35">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="15" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="D15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="35">
+        <v>0.35</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J15" s="35">
+        <v>0.6</v>
+      </c>
+      <c r="U15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="V15" s="35">
+        <v>0.35</v>
+      </c>
+      <c r="Z15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA15" s="35">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="16" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="L16" s="7"/>
+      <c r="AC16" s="7"/>
+    </row>
+    <row r="17" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="C17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L17" s="8"/>
+      <c r="T17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC17" s="8"/>
+    </row>
+    <row r="18" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="C18" s="6">
+        <v>1</v>
+      </c>
+      <c r="H18" s="6">
+        <v>1</v>
+      </c>
+      <c r="L18" s="7"/>
+      <c r="T18" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y18" s="6">
+        <v>1</v>
+      </c>
+      <c r="AC18" s="7"/>
+    </row>
+    <row r="19" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="L19" s="7"/>
+    </row>
+    <row r="22" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B22" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="C24" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="35">
+        <f>E5-0.5*G25*C25</f>
+        <v>0.15001742737205112</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J24" s="35">
+        <f>J5-0.5*L$25*H6</f>
+        <v>0.39948543562022693</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N24" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="C25" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="G25" s="6">
+        <f>H6*(1-H6)*H25</f>
+        <v>-6.9709488204534214E-4</v>
+      </c>
+      <c r="H25" s="6">
+        <f>J5*L25+J7*L31</f>
+        <v>-2.8889052426317322E-3</v>
+      </c>
+      <c r="L25" s="6">
+        <f>M25*N25</f>
+        <v>1.7346718580708166E-3</v>
+      </c>
+      <c r="M25" s="6">
+        <f>M6*(1-M6)</f>
+        <v>0.18681560180895948</v>
+      </c>
+      <c r="N25" s="6">
+        <f>-(O6-M6)+-(AD6-AF6)</f>
+        <v>9.2854763803117413E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="D26" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="35">
+        <f>E7-0.5*G31*C25</f>
+        <v>0.25001901116113895</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J26" s="35">
+        <f>J7-0.5*L$31*H6</f>
+        <v>0.50212555229431299</v>
+      </c>
+    </row>
+    <row r="29" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="D29" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="35">
+        <f>E10-0.5*G25*C31</f>
+        <v>0.20003485474410229</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J29" s="35">
+        <f>J10-0.5*L$25*H12</f>
+        <v>0.44948230073325535</v>
+      </c>
+    </row>
+    <row r="30" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="C30" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M30" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N30" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="C31" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="35">
+        <f>E12-0.5*G31*C31</f>
+        <v>0.30003802232227783</v>
+      </c>
+      <c r="G31" s="6">
+        <f>H12*(1-H12)*H31</f>
+        <v>-7.6044644555691928E-4</v>
+      </c>
+      <c r="H31" s="6">
+        <f>J10*L25+J12*L31</f>
+        <v>-3.1604490483141978E-3</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J31" s="35">
+        <f>J12-0.5*L$31*H12</f>
+        <v>0.5521385018229954</v>
+      </c>
+      <c r="L31" s="6">
+        <f>M31*N31</f>
+        <v>-7.165547971720118E-3</v>
+      </c>
+      <c r="M31" s="6">
+        <f>M12*(1-M12)</f>
+        <v>0.17551005281727122</v>
+      </c>
+      <c r="N31" s="6">
+        <f>-(O12-M12)+-(AD12-AF12)</f>
+        <v>-4.0826994560706931E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="D33" s="35">
+        <f>D14-0.5*G25*C18</f>
+        <v>0.35034854744102267</v>
+      </c>
+      <c r="I33" s="35">
+        <f>I14-0.5*L25*H18</f>
+        <v>0.59913266407096455</v>
+      </c>
+    </row>
+    <row r="34" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="D34" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E34" s="35">
+        <f>E15-0.5*G$31*C18</f>
+        <v>0.35038022322277845</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J34" s="35">
+        <f>J15-0.5*L$31*H18</f>
+        <v>0.60358277398586002</v>
+      </c>
+    </row>
+    <row r="35" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="L35" s="7"/>
+    </row>
+    <row r="36" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C36" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L36" s="8"/>
+    </row>
+    <row r="37" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C37" s="6">
+        <v>1</v>
+      </c>
+      <c r="H37" s="6">
+        <v>1</v>
+      </c>
+      <c r="L37" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E61986C2-8653-4DD1-B246-0EFA6CD3A7C8}">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18522,11 +18954,11 @@
       <c r="A23" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="B23" s="18" t="s">
-        <v>75</v>
+      <c r="B23" t="s">
+        <v>105</v>
       </c>
       <c r="C23" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -18585,7 +19017,7 @@
         <v>69</v>
       </c>
       <c r="C31" t="s">
-        <v>69</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -18618,7 +19050,7 @@
         <v>75</v>
       </c>
       <c r="C37" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.3">
@@ -18662,7 +19094,7 @@
         <v>69</v>
       </c>
       <c r="C45" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.3">
@@ -18701,7 +19133,7 @@
         <v>75</v>
       </c>
       <c r="C51" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.3">
@@ -19274,10 +19706,10 @@
       <c r="J2" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="K2" s="35">
+      <c r="K2" s="36">
         <v>1199908899</v>
       </c>
-      <c r="L2" s="35"/>
+      <c r="L2" s="36"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.3">
       <c r="C5" s="3" t="s">
@@ -20896,8 +21328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B03F0FE1-5CF0-446F-BF3A-D863A02C42EC}">
   <dimension ref="B2:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21118,7 +21550,7 @@
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
       <c r="L16" s="7"/>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C17" s="3" t="s">
         <v>2</v>
       </c>
@@ -21127,7 +21559,7 @@
       </c>
       <c r="L17" s="8"/>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C18" s="6">
         <v>1</v>
       </c>
@@ -21136,15 +21568,15 @@
       </c>
       <c r="L18" s="7"/>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
       <c r="L19" s="7"/>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B22" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C24" s="3" t="s">
         <v>0</v>
       </c>
@@ -21180,8 +21612,9 @@
       <c r="O24" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="Q24" s="35"/>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C25" s="6">
         <v>0.05</v>
       </c>
@@ -21208,8 +21641,9 @@
       <c r="O25" s="6">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="Q25" s="35"/>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.3">
       <c r="D26" s="4" t="s">
         <v>10</v>
       </c>
@@ -21224,8 +21658,15 @@
         <f>J7-0.5*L$31*H6</f>
         <v>0.5113012702387375</v>
       </c>
-    </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="Q26" s="35"/>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="Q27" s="35"/>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="Q28" s="35"/>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
       <c r="D29" s="4" t="s">
         <v>9</v>
       </c>
@@ -21240,8 +21681,9 @@
         <f>J10-0.5*L$25*H12</f>
         <v>0.4086661860762334</v>
       </c>
-    </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="Q29" s="35"/>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C30" s="3" t="s">
         <v>1</v>
       </c>
@@ -21263,8 +21705,9 @@
       <c r="O30" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="Q30" s="35"/>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C31" s="6">
         <v>0.1</v>
       </c>
@@ -21305,6 +21748,7 @@
       <c r="O31" s="6">
         <v>0.99</v>
       </c>
+      <c r="Q31" s="35"/>
     </row>
     <row r="33" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D33" s="5">
@@ -21365,7 +21809,7 @@
   <dimension ref="B2:AH37"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>